<commit_message>
Running with tentative parameter values specific to Barbados.
</commit_message>
<xml_diff>
--- a/GLCS_two_sector_parameters.xlsx
+++ b/GLCS_two_sector_parameters.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eric\Documents\SEI\projects\GoLoCarSce\two sector WORKING\scenario\_JM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eric\Documents\SEI\projects\GoLoCarSce\two sector WORKING\scenario\_BB\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15336" windowHeight="7680" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15336" windowHeight="7680" firstSheet="1" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Initial Values" sheetId="4" r:id="rId1"/>
@@ -297,7 +297,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" readingOrder="1"/>
@@ -324,6 +324,10 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" readingOrder="1"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -631,7 +635,7 @@
   <dimension ref="B2:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -645,7 +649,7 @@
         <v>16</v>
       </c>
       <c r="C2" s="10">
-        <v>200000</v>
+        <v>2264</v>
       </c>
       <c r="D2" t="s">
         <v>34</v>
@@ -656,7 +660,7 @@
         <v>17</v>
       </c>
       <c r="C3" s="10">
-        <v>3435105</v>
+        <v>27881.146229999998</v>
       </c>
       <c r="D3" t="s">
         <v>35</v>
@@ -667,7 +671,7 @@
         <v>37</v>
       </c>
       <c r="C4" s="10">
-        <v>11967.81551</v>
+        <v>421.87605600000001</v>
       </c>
       <c r="D4" t="s">
         <v>36</v>
@@ -678,7 +682,7 @@
         <v>18</v>
       </c>
       <c r="C5" s="10">
-        <v>2752.3580000000002</v>
+        <v>279.56599999999997</v>
       </c>
       <c r="D5" t="s">
         <v>38</v>
@@ -689,7 +693,7 @@
         <v>33</v>
       </c>
       <c r="C6" s="9">
-        <v>0.996</v>
+        <v>1.0369999999999999</v>
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.3">
@@ -697,7 +701,7 @@
         <v>54</v>
       </c>
       <c r="C7" s="10">
-        <v>200000</v>
+        <v>1488</v>
       </c>
       <c r="D7" t="s">
         <v>34</v>
@@ -708,7 +712,7 @@
         <v>58</v>
       </c>
       <c r="C8" s="5">
-        <v>0.56200000000000006</v>
+        <v>0.24299999999999999</v>
       </c>
     </row>
   </sheetData>
@@ -751,7 +755,7 @@
   <dimension ref="B3:L6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L23" sqref="L23"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -796,34 +800,34 @@
         <v>0</v>
       </c>
       <c r="C4" s="7">
-        <v>-7.01</v>
+        <v>1.5469999999999999</v>
       </c>
       <c r="D4" s="7">
-        <v>-6.4</v>
+        <v>1.4470000000000001</v>
       </c>
       <c r="E4" s="7">
-        <v>-6</v>
+        <v>1.363</v>
       </c>
       <c r="F4" s="7">
-        <v>-5.8</v>
+        <v>1.2909999999999999</v>
       </c>
       <c r="G4" s="7">
-        <v>-5.3</v>
+        <v>1.226</v>
       </c>
       <c r="H4" s="7">
-        <v>-4.9000000000000004</v>
+        <v>1.167</v>
       </c>
       <c r="I4" s="7">
-        <v>-4.7</v>
+        <v>1.119</v>
       </c>
       <c r="J4" s="7">
-        <v>-4.4000000000000004</v>
+        <v>1.077</v>
       </c>
       <c r="K4" s="7">
-        <v>-4.3</v>
+        <v>1.034</v>
       </c>
       <c r="L4" s="7">
-        <v>-4.3</v>
+        <v>0.99</v>
       </c>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.3">
@@ -831,34 +835,34 @@
         <v>1</v>
       </c>
       <c r="C5" s="7">
-        <v>17.600000000000001</v>
+        <v>12.234</v>
       </c>
       <c r="D5" s="7">
-        <v>16.8</v>
+        <v>11.808999999999999</v>
       </c>
       <c r="E5" s="7">
-        <v>15.1</v>
+        <v>11.436999999999999</v>
       </c>
       <c r="F5" s="7">
-        <v>13.4</v>
+        <v>11.15</v>
       </c>
       <c r="G5" s="7">
-        <v>11.9</v>
+        <v>10.965</v>
       </c>
       <c r="H5" s="7">
-        <v>11.2</v>
+        <v>10.87</v>
       </c>
       <c r="I5" s="7">
-        <v>10.9</v>
+        <v>10.827</v>
       </c>
       <c r="J5" s="7">
-        <v>10.6</v>
+        <v>10.787000000000001</v>
       </c>
       <c r="K5" s="7">
-        <v>10.199999999999999</v>
+        <v>10.734999999999999</v>
       </c>
       <c r="L5" s="7">
-        <v>10.199999999999999</v>
+        <v>10.677</v>
       </c>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.3">
@@ -866,34 +870,34 @@
         <v>2</v>
       </c>
       <c r="C6" s="7">
-        <v>6.8259999999999996</v>
+        <v>10.481999999999999</v>
       </c>
       <c r="D6" s="7">
-        <v>7.1</v>
+        <v>10.856</v>
       </c>
       <c r="E6" s="7">
-        <v>7.3</v>
+        <v>11.363</v>
       </c>
       <c r="F6" s="7">
-        <v>7.6</v>
+        <v>11.989000000000001</v>
       </c>
       <c r="G6" s="7">
-        <v>8.1</v>
+        <v>12.701000000000001</v>
       </c>
       <c r="H6" s="7">
-        <v>8.8000000000000007</v>
+        <v>13.381</v>
       </c>
       <c r="I6" s="7">
-        <v>9.5</v>
+        <v>13.878</v>
       </c>
       <c r="J6" s="7">
-        <v>10.3</v>
+        <v>14.173</v>
       </c>
       <c r="K6" s="7">
-        <v>11</v>
+        <v>14.101000000000001</v>
       </c>
       <c r="L6" s="7">
-        <v>11</v>
+        <v>13.817</v>
       </c>
     </row>
   </sheetData>
@@ -906,7 +910,7 @@
   <dimension ref="B3:L14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -951,34 +955,34 @@
         <v>44</v>
       </c>
       <c r="C4" s="5">
-        <v>0.12</v>
+        <v>0.12966800000000001</v>
       </c>
       <c r="D4" s="5">
-        <v>0.12</v>
+        <v>0.12966800000000001</v>
       </c>
       <c r="E4" s="5">
-        <v>0.12</v>
+        <v>0.12966800000000001</v>
       </c>
       <c r="F4" s="5">
-        <v>0.12</v>
+        <v>0.12966800000000001</v>
       </c>
       <c r="G4" s="5">
-        <v>0.12</v>
+        <v>0.12966800000000001</v>
       </c>
       <c r="H4" s="5">
-        <v>0.12</v>
+        <v>0.12966800000000001</v>
       </c>
       <c r="I4" s="5">
-        <v>0.12</v>
+        <v>0.12966800000000001</v>
       </c>
       <c r="J4" s="5">
-        <v>0.12</v>
+        <v>0.12966800000000001</v>
       </c>
       <c r="K4" s="5">
-        <v>0.12</v>
+        <v>0.12966800000000001</v>
       </c>
       <c r="L4" s="5">
-        <v>0.12</v>
+        <v>0.12966800000000001</v>
       </c>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.3">
@@ -986,34 +990,34 @@
         <v>45</v>
       </c>
       <c r="C5" s="5">
-        <v>0.95</v>
+        <v>0.82702500000000001</v>
       </c>
       <c r="D5" s="5">
-        <v>0.95</v>
+        <v>0.82702500000000001</v>
       </c>
       <c r="E5" s="5">
-        <v>0.95</v>
+        <v>0.82702500000000001</v>
       </c>
       <c r="F5" s="5">
-        <v>0.95</v>
+        <v>0.82702500000000001</v>
       </c>
       <c r="G5" s="5">
-        <v>0.95</v>
+        <v>0.82702500000000001</v>
       </c>
       <c r="H5" s="5">
-        <v>0.95</v>
+        <v>0.82702500000000001</v>
       </c>
       <c r="I5" s="5">
-        <v>0.95</v>
+        <v>0.82702500000000001</v>
       </c>
       <c r="J5" s="5">
-        <v>0.95</v>
+        <v>0.82702500000000001</v>
       </c>
       <c r="K5" s="5">
-        <v>0.95</v>
+        <v>0.82702500000000001</v>
       </c>
       <c r="L5" s="5">
-        <v>0.95</v>
+        <v>0.82702500000000001</v>
       </c>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.3">
@@ -1021,34 +1025,34 @@
         <v>46</v>
       </c>
       <c r="C6" s="5">
-        <v>2</v>
+        <v>17.558700000000002</v>
       </c>
       <c r="D6" s="5">
-        <v>2</v>
+        <v>17.558700000000002</v>
       </c>
       <c r="E6" s="5">
-        <v>2</v>
+        <v>17.558700000000002</v>
       </c>
       <c r="F6" s="5">
-        <v>2</v>
+        <v>17.558700000000002</v>
       </c>
       <c r="G6" s="5">
-        <v>2</v>
+        <v>17.558700000000002</v>
       </c>
       <c r="H6" s="5">
-        <v>2</v>
+        <v>17.558700000000002</v>
       </c>
       <c r="I6" s="5">
-        <v>2</v>
+        <v>17.558700000000002</v>
       </c>
       <c r="J6" s="5">
-        <v>2</v>
+        <v>17.558700000000002</v>
       </c>
       <c r="K6" s="5">
-        <v>2</v>
+        <v>17.558700000000002</v>
       </c>
       <c r="L6" s="5">
-        <v>2</v>
+        <v>17.558700000000002</v>
       </c>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.3">
@@ -1056,34 +1060,34 @@
         <v>47</v>
       </c>
       <c r="C7" s="5">
-        <v>0.45</v>
+        <v>0.36779699999999999</v>
       </c>
       <c r="D7" s="5">
-        <v>0.45</v>
+        <v>0.36779699999999999</v>
       </c>
       <c r="E7" s="5">
-        <v>0.45</v>
+        <v>0.36779699999999999</v>
       </c>
       <c r="F7" s="5">
-        <v>0.45</v>
+        <v>0.36779699999999999</v>
       </c>
       <c r="G7" s="5">
-        <v>0.45</v>
+        <v>0.36779699999999999</v>
       </c>
       <c r="H7" s="5">
-        <v>0.45</v>
+        <v>0.36779699999999999</v>
       </c>
       <c r="I7" s="5">
-        <v>0.45</v>
+        <v>0.36779699999999999</v>
       </c>
       <c r="J7" s="5">
-        <v>0.45</v>
+        <v>0.36779699999999999</v>
       </c>
       <c r="K7" s="5">
-        <v>0.45</v>
+        <v>0.36779699999999999</v>
       </c>
       <c r="L7" s="5">
-        <v>0.45</v>
+        <v>0.36779699999999999</v>
       </c>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.3">
@@ -1091,34 +1095,34 @@
         <v>48</v>
       </c>
       <c r="C8" s="5">
-        <v>0.42</v>
+        <v>0.55048699999999995</v>
       </c>
       <c r="D8" s="5">
-        <v>0.42</v>
+        <v>0.55048699999999995</v>
       </c>
       <c r="E8" s="5">
-        <v>0.42</v>
+        <v>0.55048699999999995</v>
       </c>
       <c r="F8" s="5">
-        <v>0.42</v>
+        <v>0.55048699999999995</v>
       </c>
       <c r="G8" s="5">
-        <v>0.42</v>
+        <v>0.55048699999999995</v>
       </c>
       <c r="H8" s="5">
-        <v>0.42</v>
+        <v>0.55048699999999995</v>
       </c>
       <c r="I8" s="5">
-        <v>0.42</v>
+        <v>0.55048699999999995</v>
       </c>
       <c r="J8" s="5">
-        <v>0.42</v>
+        <v>0.55048699999999995</v>
       </c>
       <c r="K8" s="5">
-        <v>0.42</v>
+        <v>0.55048699999999995</v>
       </c>
       <c r="L8" s="5">
-        <v>0.42</v>
+        <v>0.55048699999999995</v>
       </c>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.3">
@@ -1126,34 +1130,34 @@
         <v>49</v>
       </c>
       <c r="C9" s="5">
-        <v>0.36</v>
+        <v>1.06745</v>
       </c>
       <c r="D9" s="5">
-        <v>0.36</v>
+        <v>1.06745</v>
       </c>
       <c r="E9" s="5">
-        <v>0.36</v>
+        <v>1.06745</v>
       </c>
       <c r="F9" s="5">
-        <v>0.36</v>
+        <v>1.06745</v>
       </c>
       <c r="G9" s="5">
-        <v>0.36</v>
+        <v>1.06745</v>
       </c>
       <c r="H9" s="5">
-        <v>0.36</v>
+        <v>1.06745</v>
       </c>
       <c r="I9" s="5">
-        <v>0.36</v>
+        <v>1.06745</v>
       </c>
       <c r="J9" s="5">
-        <v>0.36</v>
+        <v>1.06745</v>
       </c>
       <c r="K9" s="5">
-        <v>0.36</v>
+        <v>1.06745</v>
       </c>
       <c r="L9" s="5">
-        <v>0.36</v>
+        <v>1.06745</v>
       </c>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.3">
@@ -1161,34 +1165,34 @@
         <v>50</v>
       </c>
       <c r="C10" s="5">
-        <v>1.2</v>
+        <v>0.25837199999999999</v>
       </c>
       <c r="D10" s="5">
-        <v>1.2</v>
+        <v>0.25837199999999999</v>
       </c>
       <c r="E10" s="5">
-        <v>1.2</v>
+        <v>0.25837199999999999</v>
       </c>
       <c r="F10" s="5">
-        <v>1.2</v>
+        <v>0.25837199999999999</v>
       </c>
       <c r="G10" s="5">
-        <v>1.2</v>
+        <v>0.25837199999999999</v>
       </c>
       <c r="H10" s="5">
-        <v>1.2</v>
+        <v>0.25837199999999999</v>
       </c>
       <c r="I10" s="5">
-        <v>1.2</v>
+        <v>0.25837199999999999</v>
       </c>
       <c r="J10" s="5">
-        <v>1.2</v>
+        <v>0.25837199999999999</v>
       </c>
       <c r="K10" s="5">
-        <v>1.2</v>
+        <v>0.25837199999999999</v>
       </c>
       <c r="L10" s="5">
-        <v>1.2</v>
+        <v>0.25837199999999999</v>
       </c>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.3">
@@ -1196,34 +1200,34 @@
         <v>51</v>
       </c>
       <c r="C11" s="5">
-        <v>1</v>
+        <v>1.09182</v>
       </c>
       <c r="D11" s="5">
-        <v>1</v>
+        <v>1.09182</v>
       </c>
       <c r="E11" s="5">
-        <v>1</v>
+        <v>1.09182</v>
       </c>
       <c r="F11" s="5">
-        <v>1</v>
+        <v>1.09182</v>
       </c>
       <c r="G11" s="5">
-        <v>1</v>
+        <v>1.09182</v>
       </c>
       <c r="H11" s="5">
-        <v>1</v>
+        <v>1.09182</v>
       </c>
       <c r="I11" s="5">
-        <v>1</v>
+        <v>1.09182</v>
       </c>
       <c r="J11" s="5">
-        <v>1</v>
+        <v>1.09182</v>
       </c>
       <c r="K11" s="5">
-        <v>1</v>
+        <v>1.09182</v>
       </c>
       <c r="L11" s="5">
-        <v>1</v>
+        <v>1.09182</v>
       </c>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.3">
@@ -1231,69 +1235,69 @@
         <v>52</v>
       </c>
       <c r="C12" s="5">
-        <v>1</v>
+        <v>0.78904700000000005</v>
       </c>
       <c r="D12" s="5">
-        <v>1</v>
+        <v>0.78904700000000005</v>
       </c>
       <c r="E12" s="5">
-        <v>1</v>
+        <v>0.78904700000000005</v>
       </c>
       <c r="F12" s="5">
-        <v>1</v>
+        <v>0.78904700000000005</v>
       </c>
       <c r="G12" s="5">
-        <v>1</v>
+        <v>0.78904700000000005</v>
       </c>
       <c r="H12" s="5">
-        <v>1</v>
+        <v>0.78904700000000005</v>
       </c>
       <c r="I12" s="5">
-        <v>1</v>
+        <v>0.78904700000000005</v>
       </c>
       <c r="J12" s="5">
-        <v>1</v>
+        <v>0.78904700000000005</v>
       </c>
       <c r="K12" s="5">
-        <v>1</v>
+        <v>0.78904700000000005</v>
       </c>
       <c r="L12" s="5">
-        <v>1</v>
+        <v>0.78904700000000005</v>
       </c>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>53</v>
       </c>
-      <c r="C13" s="5">
-        <v>1.71</v>
-      </c>
-      <c r="D13" s="5">
-        <v>1.71</v>
-      </c>
-      <c r="E13" s="5">
-        <v>1.71</v>
-      </c>
-      <c r="F13" s="5">
-        <v>1.71</v>
-      </c>
-      <c r="G13" s="5">
-        <v>1.71</v>
-      </c>
-      <c r="H13" s="5">
-        <v>1.71</v>
-      </c>
-      <c r="I13" s="5">
-        <v>1.71</v>
-      </c>
-      <c r="J13" s="5">
-        <v>1.71</v>
-      </c>
-      <c r="K13" s="5">
-        <v>1.71</v>
-      </c>
-      <c r="L13" s="5">
-        <v>1.71</v>
+      <c r="C13" s="17">
+        <v>2</v>
+      </c>
+      <c r="D13" s="17">
+        <v>2</v>
+      </c>
+      <c r="E13" s="17">
+        <v>2</v>
+      </c>
+      <c r="F13" s="17">
+        <v>2</v>
+      </c>
+      <c r="G13" s="17">
+        <v>2</v>
+      </c>
+      <c r="H13" s="17">
+        <v>2</v>
+      </c>
+      <c r="I13" s="17">
+        <v>2</v>
+      </c>
+      <c r="J13" s="17">
+        <v>2</v>
+      </c>
+      <c r="K13" s="17">
+        <v>2</v>
+      </c>
+      <c r="L13" s="17">
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.3">
@@ -1301,38 +1305,39 @@
         <v>60</v>
       </c>
       <c r="C14" s="5">
-        <v>1.43</v>
+        <v>3.30531</v>
       </c>
       <c r="D14" s="5">
-        <v>1.43</v>
+        <v>3.30531</v>
       </c>
       <c r="E14" s="5">
-        <v>1.43</v>
+        <v>3.30531</v>
       </c>
       <c r="F14" s="5">
-        <v>1.43</v>
+        <v>3.30531</v>
       </c>
       <c r="G14" s="5">
-        <v>1.43</v>
+        <v>3.30531</v>
       </c>
       <c r="H14" s="5">
-        <v>1.43</v>
+        <v>3.30531</v>
       </c>
       <c r="I14" s="5">
-        <v>1.43</v>
+        <v>3.30531</v>
       </c>
       <c r="J14" s="5">
-        <v>1.43</v>
+        <v>3.30531</v>
       </c>
       <c r="K14" s="5">
-        <v>1.43</v>
+        <v>3.30531</v>
       </c>
       <c r="L14" s="5">
-        <v>1.43</v>
+        <v>3.30531</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1341,7 +1346,7 @@
   <dimension ref="B3:L4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1386,34 +1391,34 @@
         <v>32</v>
       </c>
       <c r="C4" s="5">
-        <v>0.43</v>
+        <v>0.34882600000000002</v>
       </c>
       <c r="D4" s="5">
-        <v>0.43</v>
+        <v>0.34882600000000002</v>
       </c>
       <c r="E4" s="5">
-        <v>0.43</v>
+        <v>0.34882600000000002</v>
       </c>
       <c r="F4" s="5">
-        <v>0.43</v>
+        <v>0.34882600000000002</v>
       </c>
       <c r="G4" s="5">
-        <v>0.43</v>
+        <v>0.34882600000000002</v>
       </c>
       <c r="H4" s="5">
-        <v>0.43</v>
+        <v>0.34882600000000002</v>
       </c>
       <c r="I4" s="5">
-        <v>0.43</v>
+        <v>0.34882600000000002</v>
       </c>
       <c r="J4" s="5">
-        <v>0.43</v>
+        <v>0.34882600000000002</v>
       </c>
       <c r="K4" s="5">
-        <v>0.43</v>
+        <v>0.34882600000000002</v>
       </c>
       <c r="L4" s="5">
-        <v>0.43</v>
+        <v>0.34882600000000002</v>
       </c>
     </row>
   </sheetData>
@@ -1424,10 +1429,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:M21"/>
+  <dimension ref="B3:P21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1475,34 +1480,34 @@
         <v>64</v>
       </c>
       <c r="D4" s="6">
-        <v>0.02</v>
+        <v>2.5999999999999999E-2</v>
       </c>
       <c r="E4" s="6">
+        <v>0.03</v>
+      </c>
+      <c r="F4" s="6">
         <v>0.04</v>
       </c>
-      <c r="F4" s="6">
-        <v>0.06</v>
-      </c>
       <c r="G4" s="6">
-        <v>7.0000000000000007E-2</v>
+        <v>0.04</v>
       </c>
       <c r="H4" s="6">
-        <v>0.08</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="I4" s="6">
-        <v>0.09</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="J4" s="6">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="K4" s="6">
-        <v>0.1</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="L4" s="6">
-        <v>0.11</v>
+        <v>0.6</v>
       </c>
       <c r="M4" s="6">
-        <v>0.11</v>
+        <v>0.65</v>
       </c>
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.3">
@@ -1510,7 +1515,7 @@
         <v>65</v>
       </c>
       <c r="D5" s="6">
-        <v>0.02</v>
+        <v>2.5999999999999999E-2</v>
       </c>
       <c r="E5" s="6">
         <v>0.03</v>
@@ -1519,25 +1524,25 @@
         <v>0.04</v>
       </c>
       <c r="G5" s="6">
-        <v>0.05</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="H5" s="6">
-        <v>0.06</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="I5" s="6">
-        <v>0.06</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="J5" s="6">
-        <v>7.0000000000000007E-2</v>
+        <v>0.03</v>
       </c>
       <c r="K5" s="6">
-        <v>7.0000000000000007E-2</v>
+        <v>0.02</v>
       </c>
       <c r="L5" s="6">
-        <v>0.08</v>
+        <v>0.02</v>
       </c>
       <c r="M5" s="6">
-        <v>0.08</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.3">
@@ -1545,34 +1550,34 @@
         <v>66</v>
       </c>
       <c r="D6" s="6">
-        <v>0.02</v>
+        <v>2.5999999999999999E-2</v>
       </c>
       <c r="E6" s="6">
-        <v>0.02</v>
+        <v>2.5999999999999999E-2</v>
       </c>
       <c r="F6" s="6">
-        <v>0.02</v>
+        <v>2.5999999999999999E-2</v>
       </c>
       <c r="G6" s="6">
-        <v>0.03</v>
+        <v>2.5999999999999999E-2</v>
       </c>
       <c r="H6" s="6">
-        <v>0.03</v>
+        <v>2.5999999999999999E-2</v>
       </c>
       <c r="I6" s="6">
-        <v>0.03</v>
+        <v>2.5999999999999999E-2</v>
       </c>
       <c r="J6" s="6">
-        <v>3.5000000000000003E-2</v>
+        <v>2.5999999999999999E-2</v>
       </c>
       <c r="K6" s="6">
-        <v>3.5000000000000003E-2</v>
+        <v>2.5999999999999999E-2</v>
       </c>
       <c r="L6" s="6">
-        <v>3.5000000000000003E-2</v>
+        <v>2.5999999999999999E-2</v>
       </c>
       <c r="M6" s="6">
-        <v>3.5000000000000003E-2</v>
+        <v>2.5999999999999999E-2</v>
       </c>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.3">
@@ -1580,7 +1585,7 @@
         <v>67</v>
       </c>
       <c r="D7" s="6">
-        <v>0.02</v>
+        <v>2.5999999999999999E-2</v>
       </c>
       <c r="E7" s="6">
         <v>0.02</v>
@@ -1598,16 +1603,16 @@
         <v>0.01</v>
       </c>
       <c r="J7" s="6">
-        <v>0.01</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="K7" s="6">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
       <c r="L7" s="6">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
       <c r="M7" s="6">
-        <v>0.08</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.3">
@@ -1618,34 +1623,34 @@
         <v>64</v>
       </c>
       <c r="D8" s="6">
+        <v>0.123</v>
+      </c>
+      <c r="E8" s="6">
+        <v>0.11</v>
+      </c>
+      <c r="F8" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="G8" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="H8" s="6">
         <v>0.09</v>
       </c>
-      <c r="E8" s="6">
+      <c r="I8" s="6">
         <v>0.09</v>
       </c>
-      <c r="F8" s="6">
+      <c r="J8" s="6">
         <v>0.08</v>
       </c>
-      <c r="G8" s="6">
+      <c r="K8" s="6">
         <v>0.08</v>
       </c>
-      <c r="H8" s="6">
+      <c r="L8" s="6">
         <v>0.08</v>
       </c>
-      <c r="I8" s="6">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="J8" s="6">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="K8" s="6">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="L8" s="6">
-        <v>0.06</v>
-      </c>
       <c r="M8" s="6">
-        <v>0.06</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.3">
@@ -1653,34 +1658,34 @@
         <v>65</v>
       </c>
       <c r="D9" s="6">
-        <v>0.09</v>
+        <v>0.123</v>
       </c>
       <c r="E9" s="6">
-        <v>0.08</v>
+        <v>0.12</v>
       </c>
       <c r="F9" s="6">
-        <v>7.0000000000000007E-2</v>
+        <v>0.11</v>
       </c>
       <c r="G9" s="6">
-        <v>7.0000000000000007E-2</v>
+        <v>0.1</v>
       </c>
       <c r="H9" s="6">
-        <v>7.0000000000000007E-2</v>
+        <v>0.1</v>
       </c>
       <c r="I9" s="6">
-        <v>0.06</v>
+        <v>0.9</v>
       </c>
       <c r="J9" s="6">
-        <v>0.06</v>
+        <v>0.9</v>
       </c>
       <c r="K9" s="6">
-        <v>0.05</v>
+        <v>0.8</v>
       </c>
       <c r="L9" s="6">
-        <v>0.05</v>
+        <v>0.8</v>
       </c>
       <c r="M9" s="6">
-        <v>0.05</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.3">
@@ -1688,34 +1693,34 @@
         <v>66</v>
       </c>
       <c r="D10" s="6">
-        <v>0.09</v>
+        <v>0.123</v>
       </c>
       <c r="E10" s="6">
-        <v>0.09</v>
+        <v>0.123</v>
       </c>
       <c r="F10" s="6">
-        <v>0.09</v>
+        <v>0.123</v>
       </c>
       <c r="G10" s="6">
-        <v>0.09</v>
+        <v>0.123</v>
       </c>
       <c r="H10" s="6">
-        <v>0.1</v>
+        <v>0.123</v>
       </c>
       <c r="I10" s="6">
-        <v>0.1</v>
+        <v>0.123</v>
       </c>
       <c r="J10" s="6">
-        <v>0.1</v>
+        <v>0.123</v>
       </c>
       <c r="K10" s="6">
-        <v>0.1</v>
+        <v>0.123</v>
       </c>
       <c r="L10" s="6">
-        <v>0.1</v>
+        <v>0.123</v>
       </c>
       <c r="M10" s="6">
-        <v>0.1</v>
+        <v>0.123</v>
       </c>
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.3">
@@ -1723,10 +1728,10 @@
         <v>67</v>
       </c>
       <c r="D11" s="6">
-        <v>0.09</v>
+        <v>0.123</v>
       </c>
       <c r="E11" s="6">
-        <v>0.09</v>
+        <v>0.12</v>
       </c>
       <c r="F11" s="6">
         <v>0.25</v>
@@ -1784,7 +1789,7 @@
         <v>8.4000000000000005E-2</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>7</v>
       </c>
@@ -1795,7 +1800,7 @@
         <v>0.13200000000000001</v>
       </c>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>8</v>
       </c>
@@ -1805,8 +1810,16 @@
       <c r="D18" s="13">
         <v>8.8000000000000009E-2</v>
       </c>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="I18" s="16"/>
+      <c r="J18" s="16"/>
+      <c r="K18" s="16"/>
+      <c r="L18" s="16"/>
+      <c r="M18" s="16"/>
+      <c r="N18" s="16"/>
+      <c r="O18" s="16"/>
+      <c r="P18" s="16"/>
+    </row>
+    <row r="19" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>63</v>
       </c>
@@ -1817,7 +1830,7 @@
         <v>0.12296135428741198</v>
       </c>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
         <v>9</v>
       </c>
@@ -1828,7 +1841,7 @@
         <v>7.2000000000000008E-2</v>
       </c>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
         <v>10</v>
       </c>
@@ -1849,7 +1862,7 @@
   <dimension ref="B3:L15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1899,34 +1912,34 @@
         <v>11</v>
       </c>
       <c r="C5" s="12">
-        <v>3.5000000000000003E-2</v>
+        <v>3.4845899999999999E-2</v>
       </c>
       <c r="D5" s="12">
-        <v>3.5000000000000003E-2</v>
+        <v>3.4845899999999999E-2</v>
       </c>
       <c r="E5" s="12">
-        <v>3.5000000000000003E-2</v>
+        <v>3.4845899999999999E-2</v>
       </c>
       <c r="F5" s="12">
-        <v>3.5000000000000003E-2</v>
+        <v>3.4845899999999999E-2</v>
       </c>
       <c r="G5" s="12">
-        <v>3.5000000000000003E-2</v>
+        <v>3.4845899999999999E-2</v>
       </c>
       <c r="H5" s="12">
-        <v>3.5000000000000003E-2</v>
+        <v>3.4845899999999999E-2</v>
       </c>
       <c r="I5" s="12">
-        <v>3.5000000000000003E-2</v>
+        <v>3.4845899999999999E-2</v>
       </c>
       <c r="J5" s="12">
-        <v>3.5000000000000003E-2</v>
+        <v>3.4845899999999999E-2</v>
       </c>
       <c r="K5" s="12">
-        <v>3.5000000000000003E-2</v>
+        <v>3.4845899999999999E-2</v>
       </c>
       <c r="L5" s="12">
-        <v>3.5000000000000003E-2</v>
+        <v>3.4845899999999999E-2</v>
       </c>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.3">
@@ -1969,34 +1982,34 @@
         <v>13</v>
       </c>
       <c r="C7" s="12">
-        <v>0.46600000000000003</v>
+        <v>0.71654700000000005</v>
       </c>
       <c r="D7" s="12">
-        <v>0.46600000000000003</v>
+        <v>0.71654700000000005</v>
       </c>
       <c r="E7" s="12">
-        <v>0.46600000000000003</v>
+        <v>0.71654700000000005</v>
       </c>
       <c r="F7" s="12">
-        <v>0.46600000000000003</v>
+        <v>0.71654700000000005</v>
       </c>
       <c r="G7" s="12">
-        <v>0.46600000000000003</v>
+        <v>0.71654700000000005</v>
       </c>
       <c r="H7" s="12">
-        <v>0.46600000000000003</v>
+        <v>0.71654700000000005</v>
       </c>
       <c r="I7" s="12">
-        <v>0.46600000000000003</v>
+        <v>0.71654700000000005</v>
       </c>
       <c r="J7" s="12">
-        <v>0.46600000000000003</v>
+        <v>0.71654700000000005</v>
       </c>
       <c r="K7" s="12">
-        <v>0.46600000000000003</v>
+        <v>0.71654700000000005</v>
       </c>
       <c r="L7" s="12">
-        <v>0.46600000000000003</v>
+        <v>0.71654700000000005</v>
       </c>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.3">
@@ -2004,34 +2017,34 @@
         <v>14</v>
       </c>
       <c r="C8" s="12">
-        <v>2.9000000000000001E-2</v>
+        <v>9.99834E-2</v>
       </c>
       <c r="D8" s="12">
-        <v>2.9000000000000001E-2</v>
+        <v>9.99834E-2</v>
       </c>
       <c r="E8" s="12">
-        <v>2.9000000000000001E-2</v>
+        <v>9.99834E-2</v>
       </c>
       <c r="F8" s="12">
-        <v>2.9000000000000001E-2</v>
+        <v>9.99834E-2</v>
       </c>
       <c r="G8" s="12">
-        <v>2.9000000000000001E-2</v>
+        <v>9.99834E-2</v>
       </c>
       <c r="H8" s="12">
-        <v>2.9000000000000001E-2</v>
+        <v>9.99834E-2</v>
       </c>
       <c r="I8" s="12">
-        <v>2.9000000000000001E-2</v>
+        <v>9.99834E-2</v>
       </c>
       <c r="J8" s="12">
-        <v>2.9000000000000001E-2</v>
+        <v>9.99834E-2</v>
       </c>
       <c r="K8" s="12">
-        <v>2.9000000000000001E-2</v>
+        <v>9.99834E-2</v>
       </c>
       <c r="L8" s="12">
-        <v>2.9000000000000001E-2</v>
+        <v>9.99834E-2</v>
       </c>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.3">
@@ -2039,34 +2052,34 @@
         <v>57</v>
       </c>
       <c r="C9" s="5">
-        <v>1.7000000000000001E-2</v>
+        <v>-9.9999400000000002E-2</v>
       </c>
       <c r="D9" s="5">
-        <v>1.7000000000000001E-2</v>
+        <v>-9.9999400000000002E-2</v>
       </c>
       <c r="E9" s="5">
-        <v>1.7000000000000001E-2</v>
+        <v>-9.9999400000000002E-2</v>
       </c>
       <c r="F9" s="5">
-        <v>1.7000000000000001E-2</v>
+        <v>-9.9999400000000002E-2</v>
       </c>
       <c r="G9" s="5">
-        <v>1.7000000000000001E-2</v>
+        <v>-9.9999400000000002E-2</v>
       </c>
       <c r="H9" s="5">
-        <v>1.7000000000000001E-2</v>
+        <v>-9.9999400000000002E-2</v>
       </c>
       <c r="I9" s="5">
-        <v>1.7000000000000001E-2</v>
+        <v>-9.9999400000000002E-2</v>
       </c>
       <c r="J9" s="5">
-        <v>1.7000000000000001E-2</v>
+        <v>-9.9999400000000002E-2</v>
       </c>
       <c r="K9" s="5">
-        <v>1.7000000000000001E-2</v>
+        <v>-9.9999400000000002E-2</v>
       </c>
       <c r="L9" s="5">
-        <v>1.7000000000000001E-2</v>
+        <v>-9.9999400000000002E-2</v>
       </c>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.3">
@@ -2111,10 +2124,10 @@
         <v>29</v>
       </c>
       <c r="C13" s="5">
-        <v>0.06</v>
+        <v>0.1</v>
       </c>
       <c r="D13" s="5">
-        <v>0.06</v>
+        <v>0.08</v>
       </c>
       <c r="E13" s="5">
         <v>0.06</v>
@@ -2146,34 +2159,34 @@
         <v>55</v>
       </c>
       <c r="C14" s="5">
-        <v>0.16</v>
+        <v>7.4509099999999995E-2</v>
       </c>
       <c r="D14" s="5">
-        <v>0.16</v>
+        <v>7.4509099999999995E-2</v>
       </c>
       <c r="E14" s="5">
-        <v>0.16</v>
+        <v>7.4509099999999995E-2</v>
       </c>
       <c r="F14" s="5">
-        <v>0.16</v>
+        <v>7.4509099999999995E-2</v>
       </c>
       <c r="G14" s="5">
-        <v>0.16</v>
+        <v>7.4509099999999995E-2</v>
       </c>
       <c r="H14" s="5">
-        <v>0.16</v>
+        <v>7.4509099999999995E-2</v>
       </c>
       <c r="I14" s="5">
-        <v>0.16</v>
+        <v>7.4509099999999995E-2</v>
       </c>
       <c r="J14" s="5">
-        <v>0.16</v>
+        <v>7.4509099999999995E-2</v>
       </c>
       <c r="K14" s="5">
-        <v>0.16</v>
+        <v>7.4509099999999995E-2</v>
       </c>
       <c r="L14" s="5">
-        <v>0.16</v>
+        <v>7.4509099999999995E-2</v>
       </c>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.3">
@@ -2181,34 +2194,34 @@
         <v>59</v>
       </c>
       <c r="C15" s="5">
-        <v>1.54</v>
+        <v>3.4276800000000003E-2</v>
       </c>
       <c r="D15" s="5">
-        <v>1.54</v>
+        <v>3.4276800000000003E-2</v>
       </c>
       <c r="E15" s="5">
-        <v>1.54</v>
+        <v>3.4276800000000003E-2</v>
       </c>
       <c r="F15" s="5">
-        <v>1.54</v>
+        <v>3.4276800000000003E-2</v>
       </c>
       <c r="G15" s="5">
-        <v>1.54</v>
+        <v>3.4276800000000003E-2</v>
       </c>
       <c r="H15" s="5">
-        <v>1.54</v>
+        <v>3.4276800000000003E-2</v>
       </c>
       <c r="I15" s="5">
-        <v>1.54</v>
+        <v>3.4276800000000003E-2</v>
       </c>
       <c r="J15" s="5">
-        <v>1.54</v>
+        <v>3.4276800000000003E-2</v>
       </c>
       <c r="K15" s="5">
-        <v>1.54</v>
+        <v>3.4276800000000003E-2</v>
       </c>
       <c r="L15" s="5">
-        <v>1.54</v>
+        <v>3.4276800000000003E-2</v>
       </c>
     </row>
   </sheetData>
@@ -2220,8 +2233,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:P11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2285,43 +2298,34 @@
         <v>39</v>
       </c>
       <c r="D4" s="6">
-        <v>86</v>
+        <v>2</v>
       </c>
       <c r="E4" s="6">
-        <f>D4*(1+$N4+($O4-$N4)*MIN(1,(E$3-2010)/(2040-2010)))^5</f>
-        <v>103.01573831377762</v>
+        <v>2</v>
       </c>
       <c r="F4" s="6">
-        <f t="shared" ref="F4:M5" si="0">E4*(1+$N4+($O4-$N4)*MIN(1,(F$3-2010)/(2040-2010)))^5</f>
-        <v>114.25902083795334</v>
+        <v>2</v>
       </c>
       <c r="G4" s="6">
-        <f t="shared" si="0"/>
-        <v>117.20249659326163</v>
+        <v>2</v>
       </c>
       <c r="H4" s="6">
-        <f t="shared" si="0"/>
-        <v>111.04621028072467</v>
+        <v>2</v>
       </c>
       <c r="I4" s="6">
-        <f t="shared" si="0"/>
-        <v>97.058776065767987</v>
+        <v>2</v>
       </c>
       <c r="J4" s="6">
-        <f t="shared" si="0"/>
-        <v>78.154771457890945</v>
+        <v>2</v>
       </c>
       <c r="K4" s="6">
-        <f t="shared" si="0"/>
-        <v>62.932673883052168</v>
+        <v>2</v>
       </c>
       <c r="L4" s="6">
-        <f t="shared" si="0"/>
-        <v>50.675363361589355</v>
+        <v>2</v>
       </c>
       <c r="M4" s="6">
-        <f t="shared" si="0"/>
-        <v>40.805392388081508</v>
+        <v>2</v>
       </c>
       <c r="N4" s="14">
         <f>N9+$P$4</f>
@@ -2343,43 +2347,43 @@
         <v>15</v>
       </c>
       <c r="D5" s="6">
-        <v>1.77</v>
+        <v>1.774114081</v>
       </c>
       <c r="E5" s="6">
         <f>D5*(1+$N5+($O5-$N5)*MIN(1,(E$3-2010)/(2040-2010)))^5</f>
-        <v>2.45365040573295</v>
+        <v>2.4593535224080165</v>
       </c>
       <c r="F5" s="6">
-        <f t="shared" si="0"/>
-        <v>3.2068229500031049</v>
+        <f>E5*(1+$N5+($O5-$N5)*MIN(1,(F$3-2010)/(2040-2010)))^5</f>
+        <v>3.2142766954093034</v>
       </c>
       <c r="G5" s="6">
-        <f t="shared" si="0"/>
-        <v>3.9487105606704813</v>
+        <f t="shared" ref="F4:M5" si="0">F5*(1+$N5+($O5-$N5)*MIN(1,(G$3-2010)/(2040-2010)))^5</f>
+        <v>3.9578887047903422</v>
       </c>
       <c r="H5" s="6">
         <f t="shared" si="0"/>
-        <v>4.5776377798999057</v>
+        <v>4.5882777644282493</v>
       </c>
       <c r="I5" s="6">
         <f t="shared" si="0"/>
-        <v>4.992447588291955</v>
+        <v>5.0040517316628517</v>
       </c>
       <c r="J5" s="6">
         <f t="shared" si="0"/>
-        <v>5.1185131460728144</v>
+        <v>5.1304103086053052</v>
       </c>
       <c r="K5" s="6">
         <f t="shared" si="0"/>
-        <v>5.2477620171639368</v>
+        <v>5.2599595979590426</v>
       </c>
       <c r="L5" s="6">
         <f t="shared" si="0"/>
-        <v>5.3802745842155053</v>
+        <v>5.3927801692108197</v>
       </c>
       <c r="M5" s="6">
         <f t="shared" si="0"/>
-        <v>5.5161332596403509</v>
+        <v>5.5289546263278977</v>
       </c>
       <c r="N5" s="15">
         <v>0.08</v>
@@ -2393,43 +2397,43 @@
         <v>41</v>
       </c>
       <c r="D6" s="6">
-        <v>1.2</v>
+        <v>0.67543715599999998</v>
       </c>
       <c r="E6" s="6">
         <f t="shared" ref="E6:M6" si="1">D6*(1+$N6+($O6-$N6)*MIN(1,(E$3-2010)/(2040-2010)))^5</f>
-        <v>1.5995682256536232</v>
+        <v>0.90033984430287461</v>
       </c>
       <c r="F6" s="6">
         <f t="shared" si="1"/>
-        <v>2.0253484124352683</v>
+        <v>1.1399963096703274</v>
       </c>
       <c r="G6" s="6">
         <f t="shared" si="1"/>
-        <v>2.4346709328668377</v>
+        <v>1.3703893422428699</v>
       </c>
       <c r="H6" s="6">
         <f t="shared" si="1"/>
-        <v>2.7770748138265797</v>
+        <v>1.5631162618752121</v>
       </c>
       <c r="I6" s="6">
         <f t="shared" si="1"/>
-        <v>3.0039996488525444</v>
+        <v>1.6908441495383011</v>
       </c>
       <c r="J6" s="6">
         <f t="shared" si="1"/>
-        <v>3.07985440438252</v>
+        <v>1.7335400831585028</v>
       </c>
       <c r="K6" s="6">
         <f t="shared" si="1"/>
-        <v>3.1576245875453552</v>
+        <v>1.7773141426060899</v>
       </c>
       <c r="L6" s="6">
         <f t="shared" si="1"/>
-        <v>3.237358565289056</v>
+        <v>1.8221935519092336</v>
       </c>
       <c r="M6" s="6">
         <f t="shared" si="1"/>
-        <v>3.3191059258876749</v>
+        <v>1.8682062225369318</v>
       </c>
       <c r="N6" s="15">
         <v>7.0000000000000007E-2</v>
@@ -2443,43 +2447,43 @@
         <v>42</v>
       </c>
       <c r="D7" s="6">
-        <v>0.77</v>
+        <v>0.829262728</v>
       </c>
       <c r="E7" s="6">
         <f t="shared" ref="E7:M7" si="2">D7*(1+$N7+($O7-$N7)*MIN(1,(E$3-2010)/(2040-2010)))^5</f>
-        <v>0.91084274284380429</v>
+        <v>0.98094537364890333</v>
       </c>
       <c r="F7" s="6">
         <f t="shared" si="2"/>
-        <v>1.0474009673697933</v>
+        <v>1.1280137448193686</v>
       </c>
       <c r="G7" s="6">
         <f t="shared" si="2"/>
-        <v>1.1706566973395456</v>
+        <v>1.2607558005029376</v>
       </c>
       <c r="H7" s="6">
         <f t="shared" si="2"/>
-        <v>1.2715178964941571</v>
+        <v>1.3693797396721643</v>
       </c>
       <c r="I7" s="6">
         <f t="shared" si="2"/>
-        <v>1.3419003040739661</v>
+        <v>1.4451790998187102</v>
       </c>
       <c r="J7" s="6">
         <f t="shared" si="2"/>
-        <v>1.3757849683248464</v>
+        <v>1.4816716830837089</v>
       </c>
       <c r="K7" s="6">
         <f t="shared" si="2"/>
-        <v>1.4105252628098872</v>
+        <v>1.5190857498060313</v>
       </c>
       <c r="L7" s="6">
         <f t="shared" si="2"/>
-        <v>1.4461427932647155</v>
+        <v>1.5574445685977116</v>
       </c>
       <c r="M7" s="6">
         <f t="shared" si="2"/>
-        <v>1.4826597109968573</v>
+        <v>1.5967719956323967</v>
       </c>
       <c r="N7" s="15">
         <v>0.04</v>
@@ -2493,43 +2497,43 @@
         <v>16</v>
       </c>
       <c r="D8" s="6">
-        <v>0.93</v>
+        <v>0.91162992700000001</v>
       </c>
       <c r="E8" s="6">
         <f t="shared" ref="E8:M9" si="3">D8*(1+$N8+($O8-$N8)*MIN(1,(E$3-2010)/(2040-2010)))^5</f>
-        <v>1.1916594221078236</v>
+        <v>1.1681208515967929</v>
       </c>
       <c r="F8" s="6">
         <f t="shared" si="3"/>
-        <v>1.4614904639502906</v>
+        <v>1.4326219838303222</v>
       </c>
       <c r="G8" s="6">
         <f t="shared" si="3"/>
-        <v>1.7149295652952596</v>
+        <v>1.6810549617422144</v>
       </c>
       <c r="H8" s="6">
         <f t="shared" si="3"/>
-        <v>1.9245619331176964</v>
+        <v>1.8865465103172738</v>
       </c>
       <c r="I8" s="6">
         <f t="shared" si="3"/>
-        <v>2.0648026662071892</v>
+        <v>2.0240171009288876</v>
       </c>
       <c r="J8" s="6">
         <f t="shared" si="3"/>
-        <v>2.1169415209912152</v>
+        <v>2.0751260690800977</v>
       </c>
       <c r="K8" s="6">
         <f t="shared" si="3"/>
-        <v>2.1703969471952034</v>
+        <v>2.1275256027232112</v>
       </c>
       <c r="L8" s="6">
         <f t="shared" si="3"/>
-        <v>2.2252021898973404</v>
+        <v>2.1812482902541426</v>
       </c>
       <c r="M8" s="6">
         <f t="shared" si="3"/>
-        <v>2.2813913336556975</v>
+        <v>2.2363275429666407</v>
       </c>
       <c r="N8" s="15">
         <v>0.06</v>
@@ -2543,43 +2547,43 @@
         <v>43</v>
       </c>
       <c r="D9" s="6">
-        <v>1.8</v>
+        <v>1.0587964299999999</v>
       </c>
       <c r="E9" s="6">
         <f t="shared" si="3"/>
-        <v>2.6962040559219487</v>
+        <v>1.5859617938675996</v>
       </c>
       <c r="F9" s="6">
         <f t="shared" si="3"/>
-        <v>3.7522058252178474</v>
+        <v>2.2071234068699224</v>
       </c>
       <c r="G9" s="6">
         <f t="shared" si="3"/>
-        <v>4.8461536089288391</v>
+        <v>2.8506056335363721</v>
       </c>
       <c r="H9" s="6">
         <f t="shared" si="3"/>
-        <v>5.8022020401510686</v>
+        <v>3.4129726701392591</v>
       </c>
       <c r="I9" s="6">
         <f t="shared" si="3"/>
-        <v>6.4323113917911279</v>
+        <v>3.7836157434870978</v>
       </c>
       <c r="J9" s="6">
         <f t="shared" si="3"/>
-        <v>6.5947353149441712</v>
+        <v>3.8791567823654511</v>
       </c>
       <c r="K9" s="6">
         <f t="shared" si="3"/>
-        <v>6.761260645694815</v>
+        <v>3.9771103522006461</v>
       </c>
       <c r="L9" s="6">
         <f t="shared" si="3"/>
-        <v>6.9319909497244883</v>
+        <v>4.0775373724225528</v>
       </c>
       <c r="M9" s="6">
         <f t="shared" si="3"/>
-        <v>7.1070324078778562</v>
+        <v>4.1805003007529864</v>
       </c>
       <c r="N9" s="15">
         <v>0.1</v>

</xml_diff>

<commit_message>
Set BB-specific price trends.
</commit_message>
<xml_diff>
--- a/GLCS_two_sector_parameters.xlsx
+++ b/GLCS_two_sector_parameters.xlsx
@@ -297,7 +297,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" readingOrder="1"/>
@@ -321,13 +321,16 @@
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" readingOrder="1"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" readingOrder="1"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" readingOrder="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1269,34 +1272,34 @@
       <c r="B13" t="s">
         <v>53</v>
       </c>
-      <c r="C13" s="17">
+      <c r="C13" s="16">
         <v>2</v>
       </c>
-      <c r="D13" s="17">
+      <c r="D13" s="16">
         <v>2</v>
       </c>
-      <c r="E13" s="17">
+      <c r="E13" s="16">
         <v>2</v>
       </c>
-      <c r="F13" s="17">
+      <c r="F13" s="16">
         <v>2</v>
       </c>
-      <c r="G13" s="17">
+      <c r="G13" s="16">
         <v>2</v>
       </c>
-      <c r="H13" s="17">
+      <c r="H13" s="16">
         <v>2</v>
       </c>
-      <c r="I13" s="17">
+      <c r="I13" s="16">
         <v>2</v>
       </c>
-      <c r="J13" s="17">
+      <c r="J13" s="16">
         <v>2</v>
       </c>
-      <c r="K13" s="17">
+      <c r="K13" s="16">
         <v>2</v>
       </c>
-      <c r="L13" s="17">
+      <c r="L13" s="16">
         <v>2</v>
       </c>
     </row>
@@ -1810,14 +1813,14 @@
       <c r="D18" s="13">
         <v>8.8000000000000009E-2</v>
       </c>
-      <c r="I18" s="16"/>
-      <c r="J18" s="16"/>
-      <c r="K18" s="16"/>
-      <c r="L18" s="16"/>
-      <c r="M18" s="16"/>
-      <c r="N18" s="16"/>
-      <c r="O18" s="16"/>
-      <c r="P18" s="16"/>
+      <c r="I18" s="15"/>
+      <c r="J18" s="15"/>
+      <c r="K18" s="15"/>
+      <c r="L18" s="15"/>
+      <c r="M18" s="15"/>
+      <c r="N18" s="15"/>
+      <c r="O18" s="15"/>
+      <c r="P18" s="15"/>
     </row>
     <row r="19" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
@@ -2234,7 +2237,7 @@
   <dimension ref="B2:P11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2327,9 +2330,9 @@
       <c r="M4" s="6">
         <v>2</v>
       </c>
-      <c r="N4" s="14">
+      <c r="N4" s="17">
         <f>N9+$P$4</f>
-        <v>5.2600000000000008E-2</v>
+        <v>-2.2399999999999996E-2</v>
       </c>
       <c r="O4" s="14">
         <f>O9+$P$4</f>
@@ -2351,42 +2354,42 @@
       </c>
       <c r="E5" s="6">
         <f>D5*(1+$N5+($O5-$N5)*MIN(1,(E$3-2010)/(2040-2010)))^5</f>
-        <v>2.4593535224080165</v>
+        <v>2.2732685596965725</v>
       </c>
       <c r="F5" s="6">
         <f>E5*(1+$N5+($O5-$N5)*MIN(1,(F$3-2010)/(2040-2010)))^5</f>
-        <v>3.2142766954093034</v>
+        <v>2.7880116250983153</v>
       </c>
       <c r="G5" s="6">
-        <f t="shared" ref="F4:M5" si="0">F5*(1+$N5+($O5-$N5)*MIN(1,(G$3-2010)/(2040-2010)))^5</f>
-        <v>3.9578887047903422</v>
+        <f t="shared" ref="G5:M5" si="0">F5*(1+$N5+($O5-$N5)*MIN(1,(G$3-2010)/(2040-2010)))^5</f>
+        <v>3.2714846125951924</v>
       </c>
       <c r="H5" s="6">
         <f t="shared" si="0"/>
-        <v>4.5882777644282493</v>
+        <v>3.6713897046243931</v>
       </c>
       <c r="I5" s="6">
         <f t="shared" si="0"/>
-        <v>5.0040517316628517</v>
+        <v>3.9389198759188364</v>
       </c>
       <c r="J5" s="6">
         <f t="shared" si="0"/>
-        <v>5.1304103086053052</v>
+        <v>4.0383825387570678</v>
       </c>
       <c r="K5" s="6">
         <f t="shared" si="0"/>
-        <v>5.2599595979590426</v>
+        <v>4.1403567584714249</v>
       </c>
       <c r="L5" s="6">
         <f t="shared" si="0"/>
-        <v>5.3927801692108197</v>
+        <v>4.2449059550203323</v>
       </c>
       <c r="M5" s="6">
         <f t="shared" si="0"/>
-        <v>5.5289546263278977</v>
-      </c>
-      <c r="N5" s="15">
-        <v>0.08</v>
+        <v>4.3520951497956384</v>
+      </c>
+      <c r="N5" s="18">
+        <v>0.06</v>
       </c>
       <c r="O5" s="13">
         <v>5.0000000000000001E-3</v>
@@ -2401,42 +2404,42 @@
       </c>
       <c r="E6" s="6">
         <f t="shared" ref="E6:M6" si="1">D6*(1+$N6+($O6-$N6)*MIN(1,(E$3-2010)/(2040-2010)))^5</f>
-        <v>0.90033984430287461</v>
+        <v>0.69536858726426065</v>
       </c>
       <c r="F6" s="6">
         <f t="shared" si="1"/>
-        <v>1.1399963096703274</v>
+        <v>0.71529525671883865</v>
       </c>
       <c r="G6" s="6">
         <f t="shared" si="1"/>
-        <v>1.3703893422428699</v>
+        <v>0.73518344644254696</v>
       </c>
       <c r="H6" s="6">
         <f t="shared" si="1"/>
-        <v>1.5631162618752121</v>
+        <v>0.75499857547249438</v>
       </c>
       <c r="I6" s="6">
         <f t="shared" si="1"/>
-        <v>1.6908441495383011</v>
+        <v>0.7747052920107903</v>
       </c>
       <c r="J6" s="6">
         <f t="shared" si="1"/>
-        <v>1.7335400831585028</v>
+        <v>0.79426757143905313</v>
       </c>
       <c r="K6" s="6">
         <f t="shared" si="1"/>
-        <v>1.7773141426060899</v>
+        <v>0.81432382293692218</v>
       </c>
       <c r="L6" s="6">
         <f t="shared" si="1"/>
-        <v>1.8221935519092336</v>
+        <v>0.8348865199181652</v>
       </c>
       <c r="M6" s="6">
         <f t="shared" si="1"/>
-        <v>1.8682062225369318</v>
-      </c>
-      <c r="N6" s="15">
-        <v>7.0000000000000007E-2</v>
+        <v>0.85596845076587857</v>
+      </c>
+      <c r="N6" s="18">
+        <v>6.0000000000000001E-3</v>
       </c>
       <c r="O6" s="13">
         <v>5.0000000000000001E-3</v>
@@ -2451,42 +2454,42 @@
       </c>
       <c r="E7" s="6">
         <f t="shared" ref="E7:M7" si="2">D7*(1+$N7+($O7-$N7)*MIN(1,(E$3-2010)/(2040-2010)))^5</f>
-        <v>0.98094537364890333</v>
+        <v>0.86797383083957957</v>
       </c>
       <c r="F7" s="6">
         <f t="shared" si="2"/>
-        <v>1.1280137448193686</v>
+        <v>0.90474721069005259</v>
       </c>
       <c r="G7" s="6">
         <f t="shared" si="2"/>
-        <v>1.2607558005029376</v>
+        <v>0.93918798263409176</v>
       </c>
       <c r="H7" s="6">
         <f t="shared" si="2"/>
-        <v>1.3693797396721643</v>
+        <v>0.97091445767057161</v>
       </c>
       <c r="I7" s="6">
         <f t="shared" si="2"/>
-        <v>1.4451790998187102</v>
+        <v>0.9995651094812309</v>
       </c>
       <c r="J7" s="6">
         <f t="shared" si="2"/>
-        <v>1.4816716830837089</v>
+        <v>1.0248053810787838</v>
       </c>
       <c r="K7" s="6">
         <f t="shared" si="2"/>
-        <v>1.5190857498060313</v>
+        <v>1.0506830011634694</v>
       </c>
       <c r="L7" s="6">
         <f t="shared" si="2"/>
-        <v>1.5574445685977116</v>
+        <v>1.0772140635832668</v>
       </c>
       <c r="M7" s="6">
         <f t="shared" si="2"/>
-        <v>1.5967719956323967</v>
-      </c>
-      <c r="N7" s="15">
-        <v>0.04</v>
+        <v>1.1044150685759846</v>
+      </c>
+      <c r="N7" s="18">
+        <v>0.01</v>
       </c>
       <c r="O7" s="13">
         <v>5.0000000000000001E-3</v>
@@ -2501,42 +2504,42 @@
       </c>
       <c r="E8" s="6">
         <f t="shared" ref="E8:M9" si="3">D8*(1+$N8+($O8-$N8)*MIN(1,(E$3-2010)/(2040-2010)))^5</f>
-        <v>1.1681208515967929</v>
+        <v>0.97404768434231881</v>
       </c>
       <c r="F8" s="6">
         <f t="shared" si="3"/>
-        <v>1.4326219838303222</v>
+        <v>1.0322084776757086</v>
       </c>
       <c r="G8" s="6">
         <f t="shared" si="3"/>
-        <v>1.6810549617422144</v>
+        <v>1.084861483835591</v>
       </c>
       <c r="H8" s="6">
         <f t="shared" si="3"/>
-        <v>1.8865465103172738</v>
+        <v>1.13082372602859</v>
       </c>
       <c r="I8" s="6">
         <f t="shared" si="3"/>
-        <v>2.0240171009288876</v>
+        <v>1.1690238003245608</v>
       </c>
       <c r="J8" s="6">
         <f t="shared" si="3"/>
-        <v>2.0751260690800977</v>
+        <v>1.1985431162193578</v>
       </c>
       <c r="K8" s="6">
         <f t="shared" si="3"/>
-        <v>2.1275256027232112</v>
+        <v>1.2288078318319835</v>
       </c>
       <c r="L8" s="6">
         <f t="shared" si="3"/>
-        <v>2.1812482902541426</v>
+        <v>1.2598367694393944</v>
       </c>
       <c r="M8" s="6">
         <f t="shared" si="3"/>
-        <v>2.2363275429666407</v>
-      </c>
-      <c r="N8" s="15">
-        <v>0.06</v>
+        <v>1.2916492266046267</v>
+      </c>
+      <c r="N8" s="18">
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="O8" s="13">
         <v>5.0000000000000001E-3</v>
@@ -2551,42 +2554,42 @@
       </c>
       <c r="E9" s="6">
         <f t="shared" si="3"/>
-        <v>1.5859617938675996</v>
+        <v>1.178578702657272</v>
       </c>
       <c r="F9" s="6">
         <f t="shared" si="3"/>
-        <v>2.2071234068699224</v>
+        <v>1.2906497103283474</v>
       </c>
       <c r="G9" s="6">
         <f t="shared" si="3"/>
-        <v>2.8506056335363721</v>
+        <v>1.39039628755473</v>
       </c>
       <c r="H9" s="6">
         <f t="shared" si="3"/>
-        <v>3.4129726701392591</v>
+        <v>1.4734174295705693</v>
       </c>
       <c r="I9" s="6">
         <f t="shared" si="3"/>
-        <v>3.7836157434870978</v>
+        <v>1.5358415913261099</v>
       </c>
       <c r="J9" s="6">
         <f t="shared" si="3"/>
-        <v>3.8791567823654511</v>
+        <v>1.5746235161133866</v>
       </c>
       <c r="K9" s="6">
         <f t="shared" si="3"/>
-        <v>3.9771103522006461</v>
+        <v>1.6143847331002625</v>
       </c>
       <c r="L9" s="6">
         <f t="shared" si="3"/>
-        <v>4.0775373724225528</v>
+        <v>1.6551499706419563</v>
       </c>
       <c r="M9" s="6">
         <f t="shared" si="3"/>
-        <v>4.1805003007529864</v>
-      </c>
-      <c r="N9" s="15">
-        <v>0.1</v>
+        <v>1.6969445815156436</v>
+      </c>
+      <c r="N9" s="18">
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="O9" s="13">
         <v>5.0000000000000001E-3</v>

</xml_diff>

<commit_message>
Updated to most recent model and added revised parameter estimates.
</commit_message>
<xml_diff>
--- a/GLCS_two_sector_parameters.xlsx
+++ b/GLCS_two_sector_parameters.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15336" windowHeight="7680" firstSheet="1" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15336" windowHeight="7680" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Initial Values" sheetId="4" r:id="rId1"/>
@@ -26,8 +26,42 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Eric Kemp-Benedict</author>
+  </authors>
+  <commentList>
+    <comment ref="C6" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Eric Kemp-Benedict:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Not really constant -- can change -- need another name</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="67">
   <si>
     <t>Net migration rate</t>
   </si>
@@ -125,18 +159,9 @@
     <t>Set to 1 if climate damage is made up in the subsequent time period through additional investment</t>
   </si>
   <si>
-    <t>Import propensity</t>
-  </si>
-  <si>
     <t>Utilization</t>
   </si>
   <si>
-    <t>mln JMD/year</t>
-  </si>
-  <si>
-    <t>mln JMD</t>
-  </si>
-  <si>
     <t>mln USD</t>
   </si>
   <si>
@@ -152,18 +177,9 @@
     <t>Price levels</t>
   </si>
   <si>
-    <t>Consumption</t>
-  </si>
-  <si>
     <t>Imports</t>
   </si>
   <si>
-    <t>GDP</t>
-  </si>
-  <si>
-    <t>Production determinant</t>
-  </si>
-  <si>
     <t>Marginal expenditure on domestic goods</t>
   </si>
   <si>
@@ -176,36 +192,12 @@
     <t>Wage share -- exports</t>
   </si>
   <si>
-    <t>coeff X --&gt; Yd</t>
-  </si>
-  <si>
-    <t>coeff X --&gt; Yx</t>
-  </si>
-  <si>
-    <t>coeff N --&gt; Yd</t>
-  </si>
-  <si>
-    <t>coeff N --&gt; Yx</t>
-  </si>
-  <si>
-    <t>X production smoothing</t>
-  </si>
-  <si>
-    <t>Export production</t>
-  </si>
-  <si>
     <t>Interest bearing fraction</t>
   </si>
   <si>
     <t>Saving and debt</t>
   </si>
   <si>
-    <t>Foreign-domestic saving gap</t>
-  </si>
-  <si>
-    <t>Foreign ownership fraction</t>
-  </si>
-  <si>
     <t>Reference debt-to-GDP level</t>
   </si>
   <si>
@@ -231,17 +223,57 @@
   </si>
   <si>
     <t>CS4</t>
+  </si>
+  <si>
+    <t>Consumer price inflation</t>
+  </si>
+  <si>
+    <t>Consumption price</t>
+  </si>
+  <si>
+    <t>consumer price inflation constant</t>
+  </si>
+  <si>
+    <t>tech coeff xd</t>
+  </si>
+  <si>
+    <t>tech coeff dx</t>
+  </si>
+  <si>
+    <t>q</t>
+  </si>
+  <si>
+    <t>c x</t>
+  </si>
+  <si>
+    <t>wage smoothing</t>
+  </si>
+  <si>
+    <t>GDP price level</t>
+  </si>
+  <si>
+    <t>Wage/basic consumption</t>
+  </si>
+  <si>
+    <t>Base import propensity</t>
+  </si>
+  <si>
+    <t>Import elasticity</t>
+  </si>
+  <si>
+    <t>mln LC/year</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="166" formatCode="#,##0.000"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -263,6 +295,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -297,7 +342,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" readingOrder="1"/>
@@ -321,16 +366,10 @@
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" readingOrder="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" readingOrder="1"/>
-    </xf>
+    <xf numFmtId="166" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -635,10 +674,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D8"/>
+  <dimension ref="B2:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -652,10 +691,10 @@
         <v>16</v>
       </c>
       <c r="C2" s="10">
-        <v>2264</v>
+        <v>3084</v>
       </c>
       <c r="D2" t="s">
-        <v>34</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.3">
@@ -663,21 +702,21 @@
         <v>17</v>
       </c>
       <c r="C3" s="10">
-        <v>27881.146229999998</v>
+        <v>27920</v>
       </c>
       <c r="D3" t="s">
-        <v>35</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C4" s="10">
-        <v>421.87605600000001</v>
+        <v>421.9</v>
       </c>
       <c r="D4" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.3">
@@ -685,37 +724,53 @@
         <v>18</v>
       </c>
       <c r="C5" s="10">
-        <v>279.56599999999997</v>
+        <v>280.39999999999998</v>
       </c>
       <c r="D5" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C6" s="9">
-        <v>1.0369999999999999</v>
+        <v>0.98199999999999998</v>
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>54</v>
       </c>
-      <c r="C7" s="10">
-        <v>1488</v>
-      </c>
-      <c r="D7" t="s">
-        <v>34</v>
+      <c r="C7" s="16">
+        <v>4.9000000000000002E-2</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B8" t="s">
-        <v>58</v>
-      </c>
-      <c r="C8" s="5">
-        <v>0.24299999999999999</v>
+      <c r="C8" s="5"/>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>55</v>
+      </c>
+      <c r="C9" s="5">
+        <v>1.365</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>62</v>
+      </c>
+      <c r="C10" s="5">
+        <v>1.0589999999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>63</v>
+      </c>
+      <c r="C11" s="5">
+        <v>11.9</v>
       </c>
     </row>
   </sheetData>
@@ -758,7 +813,7 @@
   <dimension ref="B3:L6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -913,7 +968,7 @@
   <dimension ref="B3:L14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -954,402 +1009,378 @@
       </c>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B4" t="s">
-        <v>44</v>
-      </c>
-      <c r="C4" s="5">
-        <v>0.12966800000000001</v>
-      </c>
-      <c r="D4" s="5">
-        <v>0.12966800000000001</v>
-      </c>
-      <c r="E4" s="5">
-        <v>0.12966800000000001</v>
-      </c>
-      <c r="F4" s="5">
-        <v>0.12966800000000001</v>
-      </c>
-      <c r="G4" s="5">
-        <v>0.12966800000000001</v>
-      </c>
-      <c r="H4" s="5">
-        <v>0.12966800000000001</v>
-      </c>
-      <c r="I4" s="5">
-        <v>0.12966800000000001</v>
-      </c>
-      <c r="J4" s="5">
-        <v>0.12966800000000001</v>
-      </c>
-      <c r="K4" s="5">
-        <v>0.12966800000000001</v>
-      </c>
-      <c r="L4" s="5">
-        <v>0.12966800000000001</v>
-      </c>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
+      <c r="L4" s="5"/>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C5" s="5">
-        <v>0.82702500000000001</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="D5" s="5">
-        <v>0.82702500000000001</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="E5" s="5">
-        <v>0.82702500000000001</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="F5" s="5">
-        <v>0.82702500000000001</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="G5" s="5">
-        <v>0.82702500000000001</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="H5" s="5">
-        <v>0.82702500000000001</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="I5" s="5">
-        <v>0.82702500000000001</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="J5" s="5">
-        <v>0.82702500000000001</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="K5" s="5">
-        <v>0.82702500000000001</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="L5" s="5">
-        <v>0.82702500000000001</v>
+        <v>0.57999999999999996</v>
       </c>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="C6" s="5">
-        <v>17.558700000000002</v>
+        <v>2.5099999999999998</v>
       </c>
       <c r="D6" s="5">
-        <v>17.558700000000002</v>
+        <v>2.5099999999999998</v>
       </c>
       <c r="E6" s="5">
-        <v>17.558700000000002</v>
+        <v>2.5099999999999998</v>
       </c>
       <c r="F6" s="5">
-        <v>17.558700000000002</v>
+        <v>2.5099999999999998</v>
       </c>
       <c r="G6" s="5">
-        <v>17.558700000000002</v>
+        <v>2.5099999999999998</v>
       </c>
       <c r="H6" s="5">
-        <v>17.558700000000002</v>
+        <v>2.5099999999999998</v>
       </c>
       <c r="I6" s="5">
-        <v>17.558700000000002</v>
+        <v>2.5099999999999998</v>
       </c>
       <c r="J6" s="5">
-        <v>17.558700000000002</v>
+        <v>2.5099999999999998</v>
       </c>
       <c r="K6" s="5">
-        <v>17.558700000000002</v>
+        <v>2.5099999999999998</v>
       </c>
       <c r="L6" s="5">
-        <v>17.558700000000002</v>
+        <v>2.5099999999999998</v>
       </c>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="C7" s="5">
-        <v>0.36779699999999999</v>
+        <v>0.5</v>
       </c>
       <c r="D7" s="5">
-        <v>0.36779699999999999</v>
+        <v>0.5</v>
       </c>
       <c r="E7" s="5">
-        <v>0.36779699999999999</v>
+        <v>0.5</v>
       </c>
       <c r="F7" s="5">
-        <v>0.36779699999999999</v>
+        <v>0.5</v>
       </c>
       <c r="G7" s="5">
-        <v>0.36779699999999999</v>
+        <v>0.5</v>
       </c>
       <c r="H7" s="5">
-        <v>0.36779699999999999</v>
+        <v>0.5</v>
       </c>
       <c r="I7" s="5">
-        <v>0.36779699999999999</v>
+        <v>0.5</v>
       </c>
       <c r="J7" s="5">
-        <v>0.36779699999999999</v>
+        <v>0.5</v>
       </c>
       <c r="K7" s="5">
-        <v>0.36779699999999999</v>
+        <v>0.5</v>
       </c>
       <c r="L7" s="5">
-        <v>0.36779699999999999</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="C8" s="5">
-        <v>0.55048699999999995</v>
+        <v>0.7</v>
       </c>
       <c r="D8" s="5">
-        <v>0.55048699999999995</v>
+        <v>0.7</v>
       </c>
       <c r="E8" s="5">
-        <v>0.55048699999999995</v>
+        <v>0.7</v>
       </c>
       <c r="F8" s="5">
-        <v>0.55048699999999995</v>
+        <v>0.7</v>
       </c>
       <c r="G8" s="5">
-        <v>0.55048699999999995</v>
+        <v>0.7</v>
       </c>
       <c r="H8" s="5">
-        <v>0.55048699999999995</v>
+        <v>0.7</v>
       </c>
       <c r="I8" s="5">
-        <v>0.55048699999999995</v>
+        <v>0.7</v>
       </c>
       <c r="J8" s="5">
-        <v>0.55048699999999995</v>
+        <v>0.7</v>
       </c>
       <c r="K8" s="5">
-        <v>0.55048699999999995</v>
+        <v>0.7</v>
       </c>
       <c r="L8" s="5">
-        <v>0.55048699999999995</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="C9" s="5">
-        <v>1.06745</v>
+        <v>0.375</v>
       </c>
       <c r="D9" s="5">
-        <v>1.06745</v>
+        <v>0.375</v>
       </c>
       <c r="E9" s="5">
-        <v>1.06745</v>
+        <v>0.375</v>
       </c>
       <c r="F9" s="5">
-        <v>1.06745</v>
+        <v>0.375</v>
       </c>
       <c r="G9" s="5">
-        <v>1.06745</v>
+        <v>0.375</v>
       </c>
       <c r="H9" s="5">
-        <v>1.06745</v>
+        <v>0.375</v>
       </c>
       <c r="I9" s="5">
-        <v>1.06745</v>
+        <v>0.375</v>
       </c>
       <c r="J9" s="5">
-        <v>1.06745</v>
+        <v>0.375</v>
       </c>
       <c r="K9" s="5">
-        <v>1.06745</v>
+        <v>0.375</v>
       </c>
       <c r="L9" s="5">
-        <v>1.06745</v>
+        <v>0.375</v>
       </c>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="C10" s="5">
-        <v>0.25837199999999999</v>
+        <v>0.32800000000000001</v>
       </c>
       <c r="D10" s="5">
-        <v>0.25837199999999999</v>
+        <v>0.32800000000000001</v>
       </c>
       <c r="E10" s="5">
-        <v>0.25837199999999999</v>
+        <v>0.32800000000000001</v>
       </c>
       <c r="F10" s="5">
-        <v>0.25837199999999999</v>
+        <v>0.32800000000000001</v>
       </c>
       <c r="G10" s="5">
-        <v>0.25837199999999999</v>
+        <v>0.32800000000000001</v>
       </c>
       <c r="H10" s="5">
-        <v>0.25837199999999999</v>
+        <v>0.32800000000000001</v>
       </c>
       <c r="I10" s="5">
-        <v>0.25837199999999999</v>
+        <v>0.32800000000000001</v>
       </c>
       <c r="J10" s="5">
-        <v>0.25837199999999999</v>
+        <v>0.32800000000000001</v>
       </c>
       <c r="K10" s="5">
-        <v>0.25837199999999999</v>
+        <v>0.32800000000000001</v>
       </c>
       <c r="L10" s="5">
-        <v>0.25837199999999999</v>
+        <v>0.32800000000000001</v>
       </c>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="C11" s="5">
-        <v>1.09182</v>
+        <v>0</v>
       </c>
       <c r="D11" s="5">
-        <v>1.09182</v>
+        <v>0</v>
       </c>
       <c r="E11" s="5">
-        <v>1.09182</v>
+        <v>0</v>
       </c>
       <c r="F11" s="5">
-        <v>1.09182</v>
+        <v>0</v>
       </c>
       <c r="G11" s="5">
-        <v>1.09182</v>
+        <v>0</v>
       </c>
       <c r="H11" s="5">
-        <v>1.09182</v>
+        <v>0</v>
       </c>
       <c r="I11" s="5">
-        <v>1.09182</v>
+        <v>0</v>
       </c>
       <c r="J11" s="5">
-        <v>1.09182</v>
+        <v>0</v>
       </c>
       <c r="K11" s="5">
-        <v>1.09182</v>
+        <v>0</v>
       </c>
       <c r="L11" s="5">
-        <v>1.09182</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="C12" s="5">
-        <v>0.78904700000000005</v>
+        <v>0</v>
       </c>
       <c r="D12" s="5">
-        <v>0.78904700000000005</v>
+        <v>0</v>
       </c>
       <c r="E12" s="5">
-        <v>0.78904700000000005</v>
+        <v>0</v>
       </c>
       <c r="F12" s="5">
-        <v>0.78904700000000005</v>
+        <v>0</v>
       </c>
       <c r="G12" s="5">
-        <v>0.78904700000000005</v>
+        <v>0</v>
       </c>
       <c r="H12" s="5">
-        <v>0.78904700000000005</v>
+        <v>0</v>
       </c>
       <c r="I12" s="5">
-        <v>0.78904700000000005</v>
+        <v>0</v>
       </c>
       <c r="J12" s="5">
-        <v>0.78904700000000005</v>
+        <v>0</v>
       </c>
       <c r="K12" s="5">
-        <v>0.78904700000000005</v>
+        <v>0</v>
       </c>
       <c r="L12" s="5">
-        <v>0.78904700000000005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
-        <v>53</v>
-      </c>
-      <c r="C13" s="16">
-        <v>2</v>
-      </c>
-      <c r="D13" s="16">
-        <v>2</v>
-      </c>
-      <c r="E13" s="16">
-        <v>2</v>
-      </c>
-      <c r="F13" s="16">
-        <v>2</v>
-      </c>
-      <c r="G13" s="16">
-        <v>2</v>
-      </c>
-      <c r="H13" s="16">
-        <v>2</v>
-      </c>
-      <c r="I13" s="16">
-        <v>2</v>
-      </c>
-      <c r="J13" s="16">
-        <v>2</v>
-      </c>
-      <c r="K13" s="16">
-        <v>2</v>
-      </c>
-      <c r="L13" s="16">
-        <v>2</v>
+        <v>61</v>
+      </c>
+      <c r="C13" s="5">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="D13" s="5">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="E13" s="5">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="F13" s="5">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="G13" s="5">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="H13" s="5">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="I13" s="5">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="J13" s="5">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="K13" s="5">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="L13" s="5">
+        <v>0.56999999999999995</v>
       </c>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="C14" s="5">
-        <v>3.30531</v>
+        <v>1</v>
       </c>
       <c r="D14" s="5">
-        <v>3.30531</v>
+        <v>1</v>
       </c>
       <c r="E14" s="5">
-        <v>3.30531</v>
+        <v>1</v>
       </c>
       <c r="F14" s="5">
-        <v>3.30531</v>
+        <v>1</v>
       </c>
       <c r="G14" s="5">
-        <v>3.30531</v>
+        <v>1</v>
       </c>
       <c r="H14" s="5">
-        <v>3.30531</v>
+        <v>1</v>
       </c>
       <c r="I14" s="5">
-        <v>3.30531</v>
+        <v>1</v>
       </c>
       <c r="J14" s="5">
-        <v>3.30531</v>
+        <v>1</v>
       </c>
       <c r="K14" s="5">
-        <v>3.30531</v>
+        <v>1</v>
       </c>
       <c r="L14" s="5">
-        <v>3.30531</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:L4"/>
+  <dimension ref="B3:L5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1391,37 +1422,72 @@
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>32</v>
+        <v>64</v>
       </c>
       <c r="C4" s="5">
-        <v>0.34882600000000002</v>
+        <v>0.45600000000000002</v>
       </c>
       <c r="D4" s="5">
-        <v>0.34882600000000002</v>
+        <v>0.45600000000000002</v>
       </c>
       <c r="E4" s="5">
-        <v>0.34882600000000002</v>
+        <v>0.45600000000000002</v>
       </c>
       <c r="F4" s="5">
-        <v>0.34882600000000002</v>
+        <v>0.45600000000000002</v>
       </c>
       <c r="G4" s="5">
-        <v>0.34882600000000002</v>
+        <v>0.45600000000000002</v>
       </c>
       <c r="H4" s="5">
-        <v>0.34882600000000002</v>
+        <v>0.45600000000000002</v>
       </c>
       <c r="I4" s="5">
-        <v>0.34882600000000002</v>
+        <v>0.45600000000000002</v>
       </c>
       <c r="J4" s="5">
-        <v>0.34882600000000002</v>
+        <v>0.45600000000000002</v>
       </c>
       <c r="K4" s="5">
-        <v>0.34882600000000002</v>
+        <v>0.45600000000000002</v>
       </c>
       <c r="L4" s="5">
-        <v>0.34882600000000002</v>
+        <v>0.45600000000000002</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C5" s="5">
+        <v>0</v>
+      </c>
+      <c r="D5" s="5">
+        <v>0</v>
+      </c>
+      <c r="E5" s="5">
+        <v>0</v>
+      </c>
+      <c r="F5" s="5">
+        <v>0</v>
+      </c>
+      <c r="G5" s="5">
+        <v>0</v>
+      </c>
+      <c r="H5" s="5">
+        <v>0</v>
+      </c>
+      <c r="I5" s="5">
+        <v>0</v>
+      </c>
+      <c r="J5" s="5">
+        <v>0</v>
+      </c>
+      <c r="K5" s="5">
+        <v>0</v>
+      </c>
+      <c r="L5" s="5">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1432,10 +1498,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:P21"/>
+  <dimension ref="B3:M21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N13" sqref="N13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4:M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1480,77 +1546,77 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="D4" s="6">
         <v>2.5999999999999999E-2</v>
       </c>
       <c r="E4" s="6">
-        <v>0.03</v>
+        <v>2.5999999999999999E-2</v>
       </c>
       <c r="F4" s="6">
-        <v>0.04</v>
+        <v>2.5999999999999999E-2</v>
       </c>
       <c r="G4" s="6">
-        <v>0.04</v>
+        <v>2.5999999999999999E-2</v>
       </c>
       <c r="H4" s="6">
-        <v>4.4999999999999998E-2</v>
+        <v>2.5999999999999999E-2</v>
       </c>
       <c r="I4" s="6">
-        <v>4.4999999999999998E-2</v>
+        <v>2.5999999999999999E-2</v>
       </c>
       <c r="J4" s="6">
-        <v>0.5</v>
+        <v>2.5999999999999999E-2</v>
       </c>
       <c r="K4" s="6">
-        <v>0.55000000000000004</v>
+        <v>2.5999999999999999E-2</v>
       </c>
       <c r="L4" s="6">
-        <v>0.6</v>
+        <v>2.5999999999999999E-2</v>
       </c>
       <c r="M4" s="6">
-        <v>0.65</v>
+        <v>2.5999999999999999E-2</v>
       </c>
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.3">
       <c r="C5" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
       <c r="D5" s="6">
         <v>2.5999999999999999E-2</v>
       </c>
       <c r="E5" s="6">
-        <v>0.03</v>
+        <v>2.5999999999999999E-2</v>
       </c>
       <c r="F5" s="6">
-        <v>0.04</v>
+        <v>2.5999999999999999E-2</v>
       </c>
       <c r="G5" s="6">
-        <v>4.4999999999999998E-2</v>
+        <v>2.5999999999999999E-2</v>
       </c>
       <c r="H5" s="6">
-        <v>4.4999999999999998E-2</v>
+        <v>2.5999999999999999E-2</v>
       </c>
       <c r="I5" s="6">
-        <v>4.4999999999999998E-2</v>
+        <v>2.5999999999999999E-2</v>
       </c>
       <c r="J5" s="6">
-        <v>0.03</v>
+        <v>2.5999999999999999E-2</v>
       </c>
       <c r="K5" s="6">
-        <v>0.02</v>
+        <v>2.5999999999999999E-2</v>
       </c>
       <c r="L5" s="6">
-        <v>0.02</v>
+        <v>2.5999999999999999E-2</v>
       </c>
       <c r="M5" s="6">
-        <v>0.02</v>
+        <v>2.5999999999999999E-2</v>
       </c>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.3">
       <c r="C6" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="D6" s="6">
         <v>2.5999999999999999E-2</v>
@@ -1585,37 +1651,37 @@
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.3">
       <c r="C7" t="s">
-        <v>67</v>
+        <v>53</v>
       </c>
       <c r="D7" s="6">
         <v>2.5999999999999999E-2</v>
       </c>
       <c r="E7" s="6">
-        <v>0.02</v>
+        <v>2.5999999999999999E-2</v>
       </c>
       <c r="F7" s="6">
-        <v>-0.02</v>
+        <v>2.5999999999999999E-2</v>
       </c>
       <c r="G7" s="6">
-        <v>-0.01</v>
+        <v>2.5999999999999999E-2</v>
       </c>
       <c r="H7" s="6">
-        <v>0</v>
+        <v>2.5999999999999999E-2</v>
       </c>
       <c r="I7" s="6">
-        <v>0.01</v>
+        <v>2.5999999999999999E-2</v>
       </c>
       <c r="J7" s="6">
-        <v>1.4999999999999999E-2</v>
+        <v>2.5999999999999999E-2</v>
       </c>
       <c r="K7" s="6">
-        <v>0.02</v>
+        <v>2.5999999999999999E-2</v>
       </c>
       <c r="L7" s="6">
-        <v>0.02</v>
+        <v>2.5999999999999999E-2</v>
       </c>
       <c r="M7" s="6">
-        <v>0.02</v>
+        <v>2.5999999999999999E-2</v>
       </c>
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.3">
@@ -1623,77 +1689,77 @@
         <v>20</v>
       </c>
       <c r="C8" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="D8" s="6">
         <v>0.123</v>
       </c>
       <c r="E8" s="6">
-        <v>0.11</v>
+        <v>0.123</v>
       </c>
       <c r="F8" s="6">
-        <v>0.1</v>
+        <v>0.123</v>
       </c>
       <c r="G8" s="6">
-        <v>0.1</v>
+        <v>0.123</v>
       </c>
       <c r="H8" s="6">
-        <v>0.09</v>
+        <v>0.123</v>
       </c>
       <c r="I8" s="6">
-        <v>0.09</v>
+        <v>0.123</v>
       </c>
       <c r="J8" s="6">
-        <v>0.08</v>
+        <v>0.123</v>
       </c>
       <c r="K8" s="6">
-        <v>0.08</v>
+        <v>0.123</v>
       </c>
       <c r="L8" s="6">
-        <v>0.08</v>
+        <v>0.123</v>
       </c>
       <c r="M8" s="6">
-        <v>0.08</v>
+        <v>0.123</v>
       </c>
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.3">
       <c r="C9" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
       <c r="D9" s="6">
         <v>0.123</v>
       </c>
       <c r="E9" s="6">
-        <v>0.12</v>
+        <v>0.123</v>
       </c>
       <c r="F9" s="6">
-        <v>0.11</v>
+        <v>0.123</v>
       </c>
       <c r="G9" s="6">
-        <v>0.1</v>
+        <v>0.123</v>
       </c>
       <c r="H9" s="6">
-        <v>0.1</v>
+        <v>0.123</v>
       </c>
       <c r="I9" s="6">
-        <v>0.9</v>
+        <v>0.123</v>
       </c>
       <c r="J9" s="6">
-        <v>0.9</v>
+        <v>0.123</v>
       </c>
       <c r="K9" s="6">
-        <v>0.8</v>
+        <v>0.123</v>
       </c>
       <c r="L9" s="6">
-        <v>0.8</v>
+        <v>0.123</v>
       </c>
       <c r="M9" s="6">
-        <v>0.8</v>
+        <v>0.123</v>
       </c>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.3">
       <c r="C10" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="D10" s="6">
         <v>0.123</v>
@@ -1728,37 +1794,37 @@
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.3">
       <c r="C11" t="s">
-        <v>67</v>
+        <v>53</v>
       </c>
       <c r="D11" s="6">
         <v>0.123</v>
       </c>
       <c r="E11" s="6">
-        <v>0.12</v>
+        <v>0.123</v>
       </c>
       <c r="F11" s="6">
-        <v>0.25</v>
+        <v>0.123</v>
       </c>
       <c r="G11" s="6">
-        <v>0.25</v>
+        <v>0.123</v>
       </c>
       <c r="H11" s="6">
-        <v>0.15</v>
+        <v>0.123</v>
       </c>
       <c r="I11" s="6">
-        <v>0.15</v>
+        <v>0.123</v>
       </c>
       <c r="J11" s="6">
-        <v>0.15</v>
+        <v>0.123</v>
       </c>
       <c r="K11" s="6">
-        <v>0.15</v>
+        <v>0.123</v>
       </c>
       <c r="L11" s="6">
-        <v>0.15</v>
+        <v>0.123</v>
       </c>
       <c r="M11" s="6">
-        <v>0.15</v>
+        <v>0.123</v>
       </c>
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.3">
@@ -1792,7 +1858,7 @@
         <v>8.4000000000000005E-2</v>
       </c>
     </row>
-    <row r="17" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>7</v>
       </c>
@@ -1803,7 +1869,7 @@
         <v>0.13200000000000001</v>
       </c>
     </row>
-    <row r="18" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>8</v>
       </c>
@@ -1813,18 +1879,10 @@
       <c r="D18" s="13">
         <v>8.8000000000000009E-2</v>
       </c>
-      <c r="I18" s="15"/>
-      <c r="J18" s="15"/>
-      <c r="K18" s="15"/>
-      <c r="L18" s="15"/>
-      <c r="M18" s="15"/>
-      <c r="N18" s="15"/>
-      <c r="O18" s="15"/>
-      <c r="P18" s="15"/>
-    </row>
-    <row r="19" spans="2:16" x14ac:dyDescent="0.3">
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
-        <v>63</v>
+        <v>49</v>
       </c>
       <c r="C19" s="13">
         <v>2.6070458371130943E-2</v>
@@ -1833,7 +1891,7 @@
         <v>0.12296135428741198</v>
       </c>
     </row>
-    <row r="20" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
         <v>9</v>
       </c>
@@ -1844,7 +1902,7 @@
         <v>7.2000000000000008E-2</v>
       </c>
     </row>
-    <row r="21" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
         <v>10</v>
       </c>
@@ -1865,7 +1923,7 @@
   <dimension ref="B3:L15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1915,34 +1973,34 @@
         <v>11</v>
       </c>
       <c r="C5" s="12">
-        <v>3.4845899999999999E-2</v>
+        <v>5.5599999999999997E-2</v>
       </c>
       <c r="D5" s="12">
-        <v>3.4845899999999999E-2</v>
+        <v>5.5599999999999997E-2</v>
       </c>
       <c r="E5" s="12">
-        <v>3.4845899999999999E-2</v>
+        <v>5.5599999999999997E-2</v>
       </c>
       <c r="F5" s="12">
-        <v>3.4845899999999999E-2</v>
+        <v>5.5599999999999997E-2</v>
       </c>
       <c r="G5" s="12">
-        <v>3.4845899999999999E-2</v>
+        <v>5.5599999999999997E-2</v>
       </c>
       <c r="H5" s="12">
-        <v>3.4845899999999999E-2</v>
+        <v>5.5599999999999997E-2</v>
       </c>
       <c r="I5" s="12">
-        <v>3.4845899999999999E-2</v>
+        <v>5.5599999999999997E-2</v>
       </c>
       <c r="J5" s="12">
-        <v>3.4845899999999999E-2</v>
+        <v>5.5599999999999997E-2</v>
       </c>
       <c r="K5" s="12">
-        <v>3.4845899999999999E-2</v>
+        <v>5.5599999999999997E-2</v>
       </c>
       <c r="L5" s="12">
-        <v>3.4845899999999999E-2</v>
+        <v>5.5599999999999997E-2</v>
       </c>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.3">
@@ -1985,34 +2043,34 @@
         <v>13</v>
       </c>
       <c r="C7" s="12">
-        <v>0.71654700000000005</v>
+        <v>0.312</v>
       </c>
       <c r="D7" s="12">
-        <v>0.71654700000000005</v>
+        <v>0.312</v>
       </c>
       <c r="E7" s="12">
-        <v>0.71654700000000005</v>
+        <v>0.312</v>
       </c>
       <c r="F7" s="12">
-        <v>0.71654700000000005</v>
+        <v>0.312</v>
       </c>
       <c r="G7" s="12">
-        <v>0.71654700000000005</v>
+        <v>0.312</v>
       </c>
       <c r="H7" s="12">
-        <v>0.71654700000000005</v>
+        <v>0.312</v>
       </c>
       <c r="I7" s="12">
-        <v>0.71654700000000005</v>
+        <v>0.312</v>
       </c>
       <c r="J7" s="12">
-        <v>0.71654700000000005</v>
+        <v>0.312</v>
       </c>
       <c r="K7" s="12">
-        <v>0.71654700000000005</v>
+        <v>0.312</v>
       </c>
       <c r="L7" s="12">
-        <v>0.71654700000000005</v>
+        <v>0.312</v>
       </c>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.3">
@@ -2020,74 +2078,51 @@
         <v>14</v>
       </c>
       <c r="C8" s="12">
-        <v>9.99834E-2</v>
+        <v>8.9499999999999996E-2</v>
       </c>
       <c r="D8" s="12">
-        <v>9.99834E-2</v>
+        <v>8.9499999999999996E-2</v>
       </c>
       <c r="E8" s="12">
-        <v>9.99834E-2</v>
+        <v>8.9499999999999996E-2</v>
       </c>
       <c r="F8" s="12">
-        <v>9.99834E-2</v>
+        <v>8.9499999999999996E-2</v>
       </c>
       <c r="G8" s="12">
-        <v>9.99834E-2</v>
+        <v>8.9499999999999996E-2</v>
       </c>
       <c r="H8" s="12">
-        <v>9.99834E-2</v>
+        <v>8.9499999999999996E-2</v>
       </c>
       <c r="I8" s="12">
-        <v>9.99834E-2</v>
+        <v>8.9499999999999996E-2</v>
       </c>
       <c r="J8" s="12">
-        <v>9.99834E-2</v>
+        <v>8.9499999999999996E-2</v>
       </c>
       <c r="K8" s="12">
-        <v>9.99834E-2</v>
+        <v>8.9499999999999996E-2</v>
       </c>
       <c r="L8" s="12">
-        <v>9.99834E-2</v>
+        <v>8.9499999999999996E-2</v>
       </c>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B9" t="s">
-        <v>57</v>
-      </c>
-      <c r="C9" s="5">
-        <v>-9.9999400000000002E-2</v>
-      </c>
-      <c r="D9" s="5">
-        <v>-9.9999400000000002E-2</v>
-      </c>
-      <c r="E9" s="5">
-        <v>-9.9999400000000002E-2</v>
-      </c>
-      <c r="F9" s="5">
-        <v>-9.9999400000000002E-2</v>
-      </c>
-      <c r="G9" s="5">
-        <v>-9.9999400000000002E-2</v>
-      </c>
-      <c r="H9" s="5">
-        <v>-9.9999400000000002E-2</v>
-      </c>
-      <c r="I9" s="5">
-        <v>-9.9999400000000002E-2</v>
-      </c>
-      <c r="J9" s="5">
-        <v>-9.9999400000000002E-2</v>
-      </c>
-      <c r="K9" s="5">
-        <v>-9.9999400000000002E-2</v>
-      </c>
-      <c r="L9" s="5">
-        <v>-9.9999400000000002E-2</v>
-      </c>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="5"/>
+      <c r="K9" s="5"/>
+      <c r="L9" s="5"/>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B11" s="2" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.3">
@@ -2159,72 +2194,72 @@
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="C14" s="5">
-        <v>7.4509099999999995E-2</v>
+        <v>0.05</v>
       </c>
       <c r="D14" s="5">
-        <v>7.4509099999999995E-2</v>
+        <v>0.05</v>
       </c>
       <c r="E14" s="5">
-        <v>7.4509099999999995E-2</v>
+        <v>0.05</v>
       </c>
       <c r="F14" s="5">
-        <v>7.4509099999999995E-2</v>
+        <v>0.05</v>
       </c>
       <c r="G14" s="5">
-        <v>7.4509099999999995E-2</v>
+        <v>0.05</v>
       </c>
       <c r="H14" s="5">
-        <v>7.4509099999999995E-2</v>
+        <v>0.05</v>
       </c>
       <c r="I14" s="5">
-        <v>7.4509099999999995E-2</v>
+        <v>0.05</v>
       </c>
       <c r="J14" s="5">
-        <v>7.4509099999999995E-2</v>
+        <v>0.05</v>
       </c>
       <c r="K14" s="5">
-        <v>7.4509099999999995E-2</v>
+        <v>0.05</v>
       </c>
       <c r="L14" s="5">
-        <v>7.4509099999999995E-2</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
       <c r="C15" s="5">
-        <v>3.4276800000000003E-2</v>
+        <v>0.18099999999999999</v>
       </c>
       <c r="D15" s="5">
-        <v>3.4276800000000003E-2</v>
+        <v>0.18099999999999999</v>
       </c>
       <c r="E15" s="5">
-        <v>3.4276800000000003E-2</v>
+        <v>0.18099999999999999</v>
       </c>
       <c r="F15" s="5">
-        <v>3.4276800000000003E-2</v>
+        <v>0.18099999999999999</v>
       </c>
       <c r="G15" s="5">
-        <v>3.4276800000000003E-2</v>
+        <v>0.18099999999999999</v>
       </c>
       <c r="H15" s="5">
-        <v>3.4276800000000003E-2</v>
+        <v>0.18099999999999999</v>
       </c>
       <c r="I15" s="5">
-        <v>3.4276800000000003E-2</v>
+        <v>0.18099999999999999</v>
       </c>
       <c r="J15" s="5">
-        <v>3.4276800000000003E-2</v>
+        <v>0.18099999999999999</v>
       </c>
       <c r="K15" s="5">
-        <v>3.4276800000000003E-2</v>
+        <v>0.18099999999999999</v>
       </c>
       <c r="L15" s="5">
-        <v>3.4276800000000003E-2</v>
+        <v>0.18099999999999999</v>
       </c>
     </row>
   </sheetData>
@@ -2233,11 +2268,11 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:P11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:O11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2246,7 +2281,7 @@
     <col min="3" max="3" width="15.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:15" x14ac:dyDescent="0.3">
       <c r="E2" s="11"/>
       <c r="F2" s="11"/>
       <c r="G2" s="11"/>
@@ -2258,7 +2293,7 @@
       <c r="M2" s="11"/>
       <c r="N2" s="11"/>
     </row>
-    <row r="3" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:15" x14ac:dyDescent="0.3">
       <c r="D3">
         <v>2010</v>
       </c>
@@ -2290,15 +2325,15 @@
         <v>2055</v>
       </c>
       <c r="N3" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="O3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="4" spans="2:16" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="2:15" x14ac:dyDescent="0.3">
       <c r="C4" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D4" s="6">
         <v>2</v>
@@ -2330,272 +2365,214 @@
       <c r="M4" s="6">
         <v>2</v>
       </c>
-      <c r="N4" s="17">
-        <f>N9+$P$4</f>
-        <v>-2.2399999999999996E-2</v>
-      </c>
-      <c r="O4" s="14">
-        <f>O9+$P$4</f>
-        <v>-4.24E-2</v>
-      </c>
-      <c r="P4">
-        <v>-4.7399999999999998E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="N4" s="14"/>
+      <c r="O4" s="14"/>
+    </row>
+    <row r="5" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C5" t="s">
         <v>15</v>
       </c>
       <c r="D5" s="6">
-        <v>1.774114081</v>
+        <v>0.53</v>
       </c>
       <c r="E5" s="6">
         <f>D5*(1+$N5+($O5-$N5)*MIN(1,(E$3-2010)/(2040-2010)))^5</f>
-        <v>2.2732685596965725</v>
+        <v>0.62694370611326788</v>
       </c>
       <c r="F5" s="6">
-        <f>E5*(1+$N5+($O5-$N5)*MIN(1,(F$3-2010)/(2040-2010)))^5</f>
-        <v>2.7880116250983153</v>
+        <f t="shared" ref="F5:M5" si="0">E5*(1+$N5+($O5-$N5)*MIN(1,(F$3-2010)/(2040-2010)))^5</f>
+        <v>0.72093832818959802</v>
       </c>
       <c r="G5" s="6">
-        <f t="shared" ref="G5:M5" si="0">F5*(1+$N5+($O5-$N5)*MIN(1,(G$3-2010)/(2040-2010)))^5</f>
-        <v>3.2714846125951924</v>
+        <f t="shared" si="0"/>
+        <v>0.80577668777916778</v>
       </c>
       <c r="H5" s="6">
         <f t="shared" si="0"/>
-        <v>3.6713897046243931</v>
+        <v>0.87520063005441995</v>
       </c>
       <c r="I5" s="6">
         <f t="shared" si="0"/>
-        <v>3.9389198759188364</v>
+        <v>0.92364566384311964</v>
       </c>
       <c r="J5" s="6">
         <f t="shared" si="0"/>
-        <v>4.0383825387570678</v>
+        <v>0.94696887430151777</v>
       </c>
       <c r="K5" s="6">
         <f t="shared" si="0"/>
-        <v>4.1403567584714249</v>
+        <v>0.97088102505096141</v>
       </c>
       <c r="L5" s="6">
         <f t="shared" si="0"/>
-        <v>4.2449059550203323</v>
+        <v>0.99539698757181716</v>
       </c>
       <c r="M5" s="6">
         <f t="shared" si="0"/>
-        <v>4.3520951497956384</v>
-      </c>
-      <c r="N5" s="18">
-        <v>0.06</v>
+        <v>1.0205320088679668</v>
+      </c>
+      <c r="N5" s="15">
+        <v>0.04</v>
       </c>
       <c r="O5" s="13">
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="6" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:15" x14ac:dyDescent="0.3">
       <c r="C6" t="s">
-        <v>41</v>
+        <v>56</v>
       </c>
       <c r="D6" s="6">
-        <v>0.67543715599999998</v>
+        <v>0.05</v>
       </c>
       <c r="E6" s="6">
-        <f t="shared" ref="E6:M6" si="1">D6*(1+$N6+($O6-$N6)*MIN(1,(E$3-2010)/(2040-2010)))^5</f>
-        <v>0.69536858726426065</v>
+        <v>0.04</v>
       </c>
       <c r="F6" s="6">
+        <v>0.03</v>
+      </c>
+      <c r="G6" s="6">
+        <v>0.02</v>
+      </c>
+      <c r="H6" s="6">
+        <v>0.02</v>
+      </c>
+      <c r="I6" s="6">
+        <v>0.02</v>
+      </c>
+      <c r="J6" s="6">
+        <v>0.02</v>
+      </c>
+      <c r="K6" s="6">
+        <v>0.02</v>
+      </c>
+      <c r="L6" s="6">
+        <v>0.02</v>
+      </c>
+      <c r="M6" s="6">
+        <v>0.02</v>
+      </c>
+      <c r="N6" s="15"/>
+      <c r="O6" s="13"/>
+    </row>
+    <row r="7" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="C7" t="s">
+        <v>38</v>
+      </c>
+      <c r="D7" s="6">
+        <v>0.78</v>
+      </c>
+      <c r="E7" s="6">
+        <f t="shared" ref="E7:M7" si="1">D7*(1+$N7+($O7-$N7)*MIN(1,(E$3-2010)/(2040-2010)))^5</f>
+        <v>0.92267186937424328</v>
+      </c>
+      <c r="F7" s="6">
         <f t="shared" si="1"/>
-        <v>0.71529525671883865</v>
-      </c>
-      <c r="G6" s="6">
+        <v>1.0610035773356348</v>
+      </c>
+      <c r="G7" s="6">
         <f t="shared" si="1"/>
-        <v>0.73518344644254696</v>
-      </c>
-      <c r="H6" s="6">
+        <v>1.1858600310712279</v>
+      </c>
+      <c r="H7" s="6">
         <f t="shared" si="1"/>
-        <v>0.75499857547249438</v>
-      </c>
-      <c r="I6" s="6">
+        <v>1.2880311159291462</v>
+      </c>
+      <c r="I7" s="6">
         <f t="shared" si="1"/>
-        <v>0.7747052920107903</v>
-      </c>
-      <c r="J6" s="6">
+        <v>1.3593275807502514</v>
+      </c>
+      <c r="J7" s="6">
         <f t="shared" si="1"/>
-        <v>0.79426757143905313</v>
-      </c>
-      <c r="K6" s="6">
+        <v>1.3936523055758183</v>
+      </c>
+      <c r="K7" s="6">
         <f t="shared" si="1"/>
-        <v>0.81432382293692218</v>
-      </c>
-      <c r="L6" s="6">
+        <v>1.4288437727165091</v>
+      </c>
+      <c r="L7" s="6">
         <f t="shared" si="1"/>
-        <v>0.8348865199181652</v>
-      </c>
-      <c r="M6" s="6">
+        <v>1.4649238685019195</v>
+      </c>
+      <c r="M7" s="6">
         <f t="shared" si="1"/>
-        <v>0.85596845076587857</v>
-      </c>
-      <c r="N6" s="18">
-        <v>6.0000000000000001E-3</v>
-      </c>
-      <c r="O6" s="13">
-        <v>5.0000000000000001E-3</v>
-      </c>
-    </row>
-    <row r="7" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="C7" t="s">
-        <v>42</v>
-      </c>
-      <c r="D7" s="6">
-        <v>0.829262728</v>
-      </c>
-      <c r="E7" s="6">
-        <f t="shared" ref="E7:M7" si="2">D7*(1+$N7+($O7-$N7)*MIN(1,(E$3-2010)/(2040-2010)))^5</f>
-        <v>0.86797383083957957</v>
-      </c>
-      <c r="F7" s="6">
-        <f t="shared" si="2"/>
-        <v>0.90474721069005259</v>
-      </c>
-      <c r="G7" s="6">
-        <f t="shared" si="2"/>
-        <v>0.93918798263409176</v>
-      </c>
-      <c r="H7" s="6">
-        <f t="shared" si="2"/>
-        <v>0.97091445767057161</v>
-      </c>
-      <c r="I7" s="6">
-        <f t="shared" si="2"/>
-        <v>0.9995651094812309</v>
-      </c>
-      <c r="J7" s="6">
-        <f t="shared" si="2"/>
-        <v>1.0248053810787838</v>
-      </c>
-      <c r="K7" s="6">
-        <f t="shared" si="2"/>
-        <v>1.0506830011634694</v>
-      </c>
-      <c r="L7" s="6">
-        <f t="shared" si="2"/>
-        <v>1.0772140635832668</v>
-      </c>
-      <c r="M7" s="6">
-        <f t="shared" si="2"/>
-        <v>1.1044150685759846</v>
-      </c>
-      <c r="N7" s="18">
-        <v>0.01</v>
+        <v>1.5019150319188943</v>
+      </c>
+      <c r="N7" s="15">
+        <v>0.04</v>
       </c>
       <c r="O7" s="13">
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="8" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:15" x14ac:dyDescent="0.3">
       <c r="C8" t="s">
         <v>16</v>
       </c>
       <c r="D8" s="6">
-        <v>0.91162992700000001</v>
+        <v>0.66</v>
       </c>
       <c r="E8" s="6">
-        <f t="shared" ref="E8:M9" si="3">D8*(1+$N8+($O8-$N8)*MIN(1,(E$3-2010)/(2040-2010)))^5</f>
-        <v>0.97404768434231881</v>
+        <f t="shared" ref="E8:M8" si="2">D8*(1+$N8+($O8-$N8)*MIN(1,(E$3-2010)/(2040-2010)))^5</f>
+        <v>0.78072235100897514</v>
       </c>
       <c r="F8" s="6">
-        <f t="shared" si="3"/>
-        <v>1.0322084776757086</v>
+        <f t="shared" si="2"/>
+        <v>0.89777225774553715</v>
       </c>
       <c r="G8" s="6">
-        <f t="shared" si="3"/>
-        <v>1.084861483835591</v>
+        <f t="shared" si="2"/>
+        <v>1.0034200262910391</v>
       </c>
       <c r="H8" s="6">
-        <f t="shared" si="3"/>
-        <v>1.13082372602859</v>
+        <f t="shared" si="2"/>
+        <v>1.0898724827092776</v>
       </c>
       <c r="I8" s="6">
-        <f t="shared" si="3"/>
-        <v>1.1690238003245608</v>
+        <f t="shared" si="2"/>
+        <v>1.1502002606348281</v>
       </c>
       <c r="J8" s="6">
-        <f t="shared" si="3"/>
-        <v>1.1985431162193578</v>
+        <f t="shared" si="2"/>
+        <v>1.179244258564154</v>
       </c>
       <c r="K8" s="6">
-        <f t="shared" si="3"/>
-        <v>1.2288078318319835</v>
+        <f t="shared" si="2"/>
+        <v>1.2090216538370462</v>
       </c>
       <c r="L8" s="6">
-        <f t="shared" si="3"/>
-        <v>1.2598367694393944</v>
+        <f t="shared" si="2"/>
+        <v>1.2395509656554704</v>
       </c>
       <c r="M8" s="6">
-        <f t="shared" si="3"/>
-        <v>1.2916492266046267</v>
-      </c>
-      <c r="N8" s="18">
-        <v>1.4999999999999999E-2</v>
+        <f t="shared" si="2"/>
+        <v>1.2708511808544491</v>
+      </c>
+      <c r="N8" s="15">
+        <v>0.04</v>
       </c>
       <c r="O8" s="13">
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="9" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="C9" t="s">
-        <v>43</v>
-      </c>
-      <c r="D9" s="6">
-        <v>1.0587964299999999</v>
-      </c>
-      <c r="E9" s="6">
-        <f t="shared" si="3"/>
-        <v>1.178578702657272</v>
-      </c>
-      <c r="F9" s="6">
-        <f t="shared" si="3"/>
-        <v>1.2906497103283474</v>
-      </c>
-      <c r="G9" s="6">
-        <f t="shared" si="3"/>
-        <v>1.39039628755473</v>
-      </c>
-      <c r="H9" s="6">
-        <f t="shared" si="3"/>
-        <v>1.4734174295705693</v>
-      </c>
-      <c r="I9" s="6">
-        <f t="shared" si="3"/>
-        <v>1.5358415913261099</v>
-      </c>
-      <c r="J9" s="6">
-        <f t="shared" si="3"/>
-        <v>1.5746235161133866</v>
-      </c>
-      <c r="K9" s="6">
-        <f t="shared" si="3"/>
-        <v>1.6143847331002625</v>
-      </c>
-      <c r="L9" s="6">
-        <f t="shared" si="3"/>
-        <v>1.6551499706419563</v>
-      </c>
-      <c r="M9" s="6">
-        <f t="shared" si="3"/>
-        <v>1.6969445815156436</v>
-      </c>
-      <c r="N9" s="18">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="O9" s="13">
-        <v>5.0000000000000001E-3</v>
-      </c>
-    </row>
-    <row r="10" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="6"/>
+      <c r="K9" s="6"/>
+      <c r="L9" s="6"/>
+      <c r="M9" s="6"/>
+      <c r="N9" s="15"/>
+      <c r="O9" s="13"/>
+    </row>
+    <row r="10" spans="2:15" x14ac:dyDescent="0.3">
       <c r="E10" s="11"/>
       <c r="F10" s="11"/>
       <c r="G10" s="11"/>
@@ -2607,11 +2584,12 @@
       <c r="M10" s="11"/>
       <c r="N10" s="11"/>
     </row>
-    <row r="11" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:15" x14ac:dyDescent="0.3">
       <c r="E11" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Removed q from the model, updated some parameters, ran scenarios.
</commit_message>
<xml_diff>
--- a/GLCS_two_sector_parameters.xlsx
+++ b/GLCS_two_sector_parameters.xlsx
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="66">
   <si>
     <t>Net migration rate</t>
   </si>
@@ -238,9 +238,6 @@
   </si>
   <si>
     <t>tech coeff dx</t>
-  </si>
-  <si>
-    <t>q</t>
   </si>
   <si>
     <t>c x</t>
@@ -677,7 +674,7 @@
   <dimension ref="B2:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -694,7 +691,7 @@
         <v>3084</v>
       </c>
       <c r="D2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.3">
@@ -705,7 +702,7 @@
         <v>27920</v>
       </c>
       <c r="D3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.3">
@@ -735,7 +732,7 @@
         <v>32</v>
       </c>
       <c r="C6" s="9">
-        <v>0.98199999999999998</v>
+        <v>0.91</v>
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.3">
@@ -759,7 +756,7 @@
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C10" s="5">
         <v>1.0589999999999999</v>
@@ -767,10 +764,11 @@
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
-        <v>63</v>
-      </c>
-      <c r="C11" s="5">
-        <v>11.9</v>
+        <v>62</v>
+      </c>
+      <c r="C11" s="12">
+        <f>6522/1322</f>
+        <v>4.9334341906202726</v>
       </c>
     </row>
   </sheetData>
@@ -968,7 +966,7 @@
   <dimension ref="B3:L14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1025,34 +1023,34 @@
         <v>39</v>
       </c>
       <c r="C5" s="5">
-        <v>0.57999999999999996</v>
+        <v>0.73</v>
       </c>
       <c r="D5" s="5">
-        <v>0.57999999999999996</v>
+        <v>0.73</v>
       </c>
       <c r="E5" s="5">
-        <v>0.57999999999999996</v>
+        <v>0.73</v>
       </c>
       <c r="F5" s="5">
-        <v>0.57999999999999996</v>
+        <v>0.73</v>
       </c>
       <c r="G5" s="5">
-        <v>0.57999999999999996</v>
+        <v>0.73</v>
       </c>
       <c r="H5" s="5">
-        <v>0.57999999999999996</v>
+        <v>0.73</v>
       </c>
       <c r="I5" s="5">
-        <v>0.57999999999999996</v>
+        <v>0.73</v>
       </c>
       <c r="J5" s="5">
-        <v>0.57999999999999996</v>
+        <v>0.73</v>
       </c>
       <c r="K5" s="5">
-        <v>0.57999999999999996</v>
+        <v>0.73</v>
       </c>
       <c r="L5" s="5">
-        <v>0.57999999999999996</v>
+        <v>0.73</v>
       </c>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.3">
@@ -1060,34 +1058,34 @@
         <v>40</v>
       </c>
       <c r="C6" s="5">
-        <v>2.5099999999999998</v>
+        <v>4.72</v>
       </c>
       <c r="D6" s="5">
-        <v>2.5099999999999998</v>
+        <v>4.72</v>
       </c>
       <c r="E6" s="5">
-        <v>2.5099999999999998</v>
+        <v>4.72</v>
       </c>
       <c r="F6" s="5">
-        <v>2.5099999999999998</v>
+        <v>4.72</v>
       </c>
       <c r="G6" s="5">
-        <v>2.5099999999999998</v>
+        <v>4.72</v>
       </c>
       <c r="H6" s="5">
-        <v>2.5099999999999998</v>
+        <v>4.72</v>
       </c>
       <c r="I6" s="5">
-        <v>2.5099999999999998</v>
+        <v>4.72</v>
       </c>
       <c r="J6" s="5">
-        <v>2.5099999999999998</v>
+        <v>4.72</v>
       </c>
       <c r="K6" s="5">
-        <v>2.5099999999999998</v>
+        <v>4.72</v>
       </c>
       <c r="L6" s="5">
-        <v>2.5099999999999998</v>
+        <v>4.72</v>
       </c>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.3">
@@ -1095,34 +1093,34 @@
         <v>41</v>
       </c>
       <c r="C7" s="5">
-        <v>0.5</v>
+        <v>0.68</v>
       </c>
       <c r="D7" s="5">
-        <v>0.5</v>
+        <v>0.68</v>
       </c>
       <c r="E7" s="5">
-        <v>0.5</v>
+        <v>0.68</v>
       </c>
       <c r="F7" s="5">
-        <v>0.5</v>
+        <v>0.68</v>
       </c>
       <c r="G7" s="5">
-        <v>0.5</v>
+        <v>0.68</v>
       </c>
       <c r="H7" s="5">
-        <v>0.5</v>
+        <v>0.68</v>
       </c>
       <c r="I7" s="5">
-        <v>0.5</v>
+        <v>0.68</v>
       </c>
       <c r="J7" s="5">
-        <v>0.5</v>
+        <v>0.68</v>
       </c>
       <c r="K7" s="5">
-        <v>0.5</v>
+        <v>0.68</v>
       </c>
       <c r="L7" s="5">
-        <v>0.5</v>
+        <v>0.68</v>
       </c>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.3">
@@ -1130,34 +1128,34 @@
         <v>42</v>
       </c>
       <c r="C8" s="5">
-        <v>0.7</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="D8" s="5">
-        <v>0.7</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="E8" s="5">
-        <v>0.7</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="F8" s="5">
-        <v>0.7</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="G8" s="5">
-        <v>0.7</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="H8" s="5">
-        <v>0.7</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="I8" s="5">
-        <v>0.7</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="J8" s="5">
-        <v>0.7</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="K8" s="5">
-        <v>0.7</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="L8" s="5">
-        <v>0.7</v>
+        <v>0.57999999999999996</v>
       </c>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.3">
@@ -1165,34 +1163,34 @@
         <v>57</v>
       </c>
       <c r="C9" s="5">
-        <v>0.375</v>
+        <v>0.20599999999999999</v>
       </c>
       <c r="D9" s="5">
-        <v>0.375</v>
+        <v>0.20599999999999999</v>
       </c>
       <c r="E9" s="5">
-        <v>0.375</v>
+        <v>0.20599999999999999</v>
       </c>
       <c r="F9" s="5">
-        <v>0.375</v>
+        <v>0.20599999999999999</v>
       </c>
       <c r="G9" s="5">
-        <v>0.375</v>
+        <v>0.20599999999999999</v>
       </c>
       <c r="H9" s="5">
-        <v>0.375</v>
+        <v>0.20599999999999999</v>
       </c>
       <c r="I9" s="5">
-        <v>0.375</v>
+        <v>0.20599999999999999</v>
       </c>
       <c r="J9" s="5">
-        <v>0.375</v>
+        <v>0.20599999999999999</v>
       </c>
       <c r="K9" s="5">
-        <v>0.375</v>
+        <v>0.20599999999999999</v>
       </c>
       <c r="L9" s="5">
-        <v>0.375</v>
+        <v>0.20599999999999999</v>
       </c>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.3">
@@ -1200,74 +1198,51 @@
         <v>58</v>
       </c>
       <c r="C10" s="5">
-        <v>0.32800000000000001</v>
+        <v>0.02</v>
       </c>
       <c r="D10" s="5">
-        <v>0.32800000000000001</v>
+        <v>0.02</v>
       </c>
       <c r="E10" s="5">
-        <v>0.32800000000000001</v>
+        <v>0.02</v>
       </c>
       <c r="F10" s="5">
-        <v>0.32800000000000001</v>
+        <v>0.02</v>
       </c>
       <c r="G10" s="5">
-        <v>0.32800000000000001</v>
+        <v>0.02</v>
       </c>
       <c r="H10" s="5">
-        <v>0.32800000000000001</v>
+        <v>0.02</v>
       </c>
       <c r="I10" s="5">
-        <v>0.32800000000000001</v>
+        <v>0.02</v>
       </c>
       <c r="J10" s="5">
-        <v>0.32800000000000001</v>
+        <v>0.02</v>
       </c>
       <c r="K10" s="5">
-        <v>0.32800000000000001</v>
+        <v>0.02</v>
       </c>
       <c r="L10" s="5">
-        <v>0.32800000000000001</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B11" t="s">
-        <v>59</v>
-      </c>
-      <c r="C11" s="5">
-        <v>0</v>
-      </c>
-      <c r="D11" s="5">
-        <v>0</v>
-      </c>
-      <c r="E11" s="5">
-        <v>0</v>
-      </c>
-      <c r="F11" s="5">
-        <v>0</v>
-      </c>
-      <c r="G11" s="5">
-        <v>0</v>
-      </c>
-      <c r="H11" s="5">
-        <v>0</v>
-      </c>
-      <c r="I11" s="5">
-        <v>0</v>
-      </c>
-      <c r="J11" s="5">
-        <v>0</v>
-      </c>
-      <c r="K11" s="5">
-        <v>0</v>
-      </c>
-      <c r="L11" s="5">
-        <v>0</v>
-      </c>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="5"/>
+      <c r="K11" s="5"/>
+      <c r="L11" s="5"/>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C12" s="5">
         <v>0</v>
@@ -1302,37 +1277,37 @@
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C13" s="5">
-        <v>0.56999999999999995</v>
+        <v>0.49</v>
       </c>
       <c r="D13" s="5">
-        <v>0.56999999999999995</v>
+        <v>0.49</v>
       </c>
       <c r="E13" s="5">
-        <v>0.56999999999999995</v>
+        <v>0.49</v>
       </c>
       <c r="F13" s="5">
-        <v>0.56999999999999995</v>
+        <v>0.49</v>
       </c>
       <c r="G13" s="5">
-        <v>0.56999999999999995</v>
+        <v>0.49</v>
       </c>
       <c r="H13" s="5">
-        <v>0.56999999999999995</v>
+        <v>0.49</v>
       </c>
       <c r="I13" s="5">
-        <v>0.56999999999999995</v>
+        <v>0.49</v>
       </c>
       <c r="J13" s="5">
-        <v>0.56999999999999995</v>
+        <v>0.49</v>
       </c>
       <c r="K13" s="5">
-        <v>0.56999999999999995</v>
+        <v>0.49</v>
       </c>
       <c r="L13" s="5">
-        <v>0.56999999999999995</v>
+        <v>0.49</v>
       </c>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.3">
@@ -1422,7 +1397,7 @@
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C4" s="5">
         <v>0.45600000000000002</v>
@@ -1457,7 +1432,7 @@
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C5" s="5">
         <v>0</v>
@@ -1501,7 +1476,7 @@
   <dimension ref="B3:M21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4:M11"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1549,34 +1524,34 @@
         <v>50</v>
       </c>
       <c r="D4" s="6">
-        <v>2.5999999999999999E-2</v>
+        <v>0.06</v>
       </c>
       <c r="E4" s="6">
-        <v>2.5999999999999999E-2</v>
+        <v>0.05</v>
       </c>
       <c r="F4" s="6">
-        <v>2.5999999999999999E-2</v>
+        <v>0.03</v>
       </c>
       <c r="G4" s="6">
-        <v>2.5999999999999999E-2</v>
+        <v>0.01</v>
       </c>
       <c r="H4" s="6">
-        <v>2.5999999999999999E-2</v>
+        <v>0.01</v>
       </c>
       <c r="I4" s="6">
-        <v>2.5999999999999999E-2</v>
+        <v>0.03</v>
       </c>
       <c r="J4" s="6">
-        <v>2.5999999999999999E-2</v>
+        <v>0.03</v>
       </c>
       <c r="K4" s="6">
-        <v>2.5999999999999999E-2</v>
+        <v>0.04</v>
       </c>
       <c r="L4" s="6">
-        <v>2.5999999999999999E-2</v>
+        <v>0.05</v>
       </c>
       <c r="M4" s="6">
-        <v>2.5999999999999999E-2</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.3">
@@ -1584,34 +1559,34 @@
         <v>51</v>
       </c>
       <c r="D5" s="6">
-        <v>2.5999999999999999E-2</v>
+        <v>0.06</v>
       </c>
       <c r="E5" s="6">
-        <v>2.5999999999999999E-2</v>
+        <v>0.04</v>
       </c>
       <c r="F5" s="6">
-        <v>2.5999999999999999E-2</v>
+        <v>0.02</v>
       </c>
       <c r="G5" s="6">
-        <v>2.5999999999999999E-2</v>
+        <v>0</v>
       </c>
       <c r="H5" s="6">
-        <v>2.5999999999999999E-2</v>
+        <v>0</v>
       </c>
       <c r="I5" s="6">
-        <v>2.5999999999999999E-2</v>
+        <v>0.02</v>
       </c>
       <c r="J5" s="6">
-        <v>2.5999999999999999E-2</v>
+        <v>0.03</v>
       </c>
       <c r="K5" s="6">
-        <v>2.5999999999999999E-2</v>
+        <v>0.04</v>
       </c>
       <c r="L5" s="6">
-        <v>2.5999999999999999E-2</v>
+        <v>0.04</v>
       </c>
       <c r="M5" s="6">
-        <v>2.5999999999999999E-2</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.3">
@@ -1619,34 +1594,34 @@
         <v>52</v>
       </c>
       <c r="D6" s="6">
-        <v>2.5999999999999999E-2</v>
+        <v>0.06</v>
       </c>
       <c r="E6" s="6">
-        <v>2.5999999999999999E-2</v>
+        <v>0.06</v>
       </c>
       <c r="F6" s="6">
-        <v>2.5999999999999999E-2</v>
+        <v>0.06</v>
       </c>
       <c r="G6" s="6">
-        <v>2.5999999999999999E-2</v>
+        <v>0.05</v>
       </c>
       <c r="H6" s="6">
-        <v>2.5999999999999999E-2</v>
+        <v>0.05</v>
       </c>
       <c r="I6" s="6">
-        <v>2.5999999999999999E-2</v>
+        <v>0.04</v>
       </c>
       <c r="J6" s="6">
-        <v>2.5999999999999999E-2</v>
+        <v>0.04</v>
       </c>
       <c r="K6" s="6">
-        <v>2.5999999999999999E-2</v>
+        <v>0.04</v>
       </c>
       <c r="L6" s="6">
-        <v>2.5999999999999999E-2</v>
+        <v>0.04</v>
       </c>
       <c r="M6" s="6">
-        <v>2.5999999999999999E-2</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.3">
@@ -1654,34 +1629,34 @@
         <v>53</v>
       </c>
       <c r="D7" s="6">
-        <v>2.5999999999999999E-2</v>
+        <v>0.06</v>
       </c>
       <c r="E7" s="6">
-        <v>2.5999999999999999E-2</v>
+        <v>0.05</v>
       </c>
       <c r="F7" s="6">
-        <v>2.5999999999999999E-2</v>
+        <v>-0.04</v>
       </c>
       <c r="G7" s="6">
-        <v>2.5999999999999999E-2</v>
+        <v>0</v>
       </c>
       <c r="H7" s="6">
-        <v>2.5999999999999999E-2</v>
+        <v>0.04</v>
       </c>
       <c r="I7" s="6">
-        <v>2.5999999999999999E-2</v>
+        <v>0.05</v>
       </c>
       <c r="J7" s="6">
-        <v>2.5999999999999999E-2</v>
+        <v>0.06</v>
       </c>
       <c r="K7" s="6">
-        <v>2.5999999999999999E-2</v>
+        <v>0.06</v>
       </c>
       <c r="L7" s="6">
-        <v>2.5999999999999999E-2</v>
+        <v>0.06</v>
       </c>
       <c r="M7" s="6">
-        <v>2.5999999999999999E-2</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.3">
@@ -1692,34 +1667,34 @@
         <v>50</v>
       </c>
       <c r="D8" s="6">
-        <v>0.123</v>
+        <v>0.13200000000000001</v>
       </c>
       <c r="E8" s="6">
-        <v>0.123</v>
+        <v>0.13</v>
       </c>
       <c r="F8" s="6">
-        <v>0.123</v>
+        <v>0.12</v>
       </c>
       <c r="G8" s="6">
-        <v>0.123</v>
+        <v>0.1</v>
       </c>
       <c r="H8" s="6">
-        <v>0.123</v>
+        <v>0.09</v>
       </c>
       <c r="I8" s="6">
-        <v>0.123</v>
+        <v>0.09</v>
       </c>
       <c r="J8" s="6">
-        <v>0.123</v>
+        <v>0.09</v>
       </c>
       <c r="K8" s="6">
-        <v>0.123</v>
+        <v>0.09</v>
       </c>
       <c r="L8" s="6">
-        <v>0.123</v>
+        <v>0.09</v>
       </c>
       <c r="M8" s="6">
-        <v>0.123</v>
+        <v>0.09</v>
       </c>
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.3">
@@ -1727,34 +1702,34 @@
         <v>51</v>
       </c>
       <c r="D9" s="6">
-        <v>0.123</v>
+        <v>0.13200000000000001</v>
       </c>
       <c r="E9" s="6">
-        <v>0.123</v>
+        <v>0.1</v>
       </c>
       <c r="F9" s="6">
-        <v>0.123</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="G9" s="6">
-        <v>0.123</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="H9" s="6">
-        <v>0.123</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="I9" s="6">
-        <v>0.123</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="J9" s="6">
-        <v>0.123</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="K9" s="6">
-        <v>0.123</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="L9" s="6">
-        <v>0.123</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="M9" s="6">
-        <v>0.123</v>
+        <v>7.0000000000000007E-2</v>
       </c>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.3">
@@ -1762,34 +1737,34 @@
         <v>52</v>
       </c>
       <c r="D10" s="6">
-        <v>0.123</v>
+        <v>0.13200000000000001</v>
       </c>
       <c r="E10" s="6">
-        <v>0.123</v>
+        <v>0.13</v>
       </c>
       <c r="F10" s="6">
-        <v>0.123</v>
+        <v>0.15</v>
       </c>
       <c r="G10" s="6">
-        <v>0.123</v>
+        <v>0.17</v>
       </c>
       <c r="H10" s="6">
-        <v>0.123</v>
+        <v>0.19</v>
       </c>
       <c r="I10" s="6">
-        <v>0.123</v>
+        <v>0.2</v>
       </c>
       <c r="J10" s="6">
-        <v>0.123</v>
+        <v>0.2</v>
       </c>
       <c r="K10" s="6">
-        <v>0.123</v>
+        <v>0.2</v>
       </c>
       <c r="L10" s="6">
-        <v>0.123</v>
+        <v>0.2</v>
       </c>
       <c r="M10" s="6">
-        <v>0.123</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.3">
@@ -1797,34 +1772,34 @@
         <v>53</v>
       </c>
       <c r="D11" s="6">
-        <v>0.123</v>
+        <v>0.13200000000000001</v>
       </c>
       <c r="E11" s="6">
-        <v>0.123</v>
+        <v>0.13</v>
       </c>
       <c r="F11" s="6">
-        <v>0.123</v>
+        <v>0.25</v>
       </c>
       <c r="G11" s="6">
-        <v>0.123</v>
+        <v>0.2</v>
       </c>
       <c r="H11" s="6">
-        <v>0.123</v>
+        <v>0.15</v>
       </c>
       <c r="I11" s="6">
-        <v>0.123</v>
+        <v>0.15</v>
       </c>
       <c r="J11" s="6">
-        <v>0.123</v>
+        <v>0.15</v>
       </c>
       <c r="K11" s="6">
-        <v>0.123</v>
+        <v>0.15</v>
       </c>
       <c r="L11" s="6">
-        <v>0.123</v>
+        <v>0.15</v>
       </c>
       <c r="M11" s="6">
-        <v>0.123</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.3">
@@ -1923,7 +1898,7 @@
   <dimension ref="B3:L15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1973,34 +1948,34 @@
         <v>11</v>
       </c>
       <c r="C5" s="12">
-        <v>5.5599999999999997E-2</v>
+        <v>5.8000000000000003E-2</v>
       </c>
       <c r="D5" s="12">
-        <v>5.5599999999999997E-2</v>
+        <v>5.8000000000000003E-2</v>
       </c>
       <c r="E5" s="12">
-        <v>5.5599999999999997E-2</v>
+        <v>5.8000000000000003E-2</v>
       </c>
       <c r="F5" s="12">
-        <v>5.5599999999999997E-2</v>
+        <v>5.8000000000000003E-2</v>
       </c>
       <c r="G5" s="12">
-        <v>5.5599999999999997E-2</v>
+        <v>5.8000000000000003E-2</v>
       </c>
       <c r="H5" s="12">
-        <v>5.5599999999999997E-2</v>
+        <v>5.8000000000000003E-2</v>
       </c>
       <c r="I5" s="12">
-        <v>5.5599999999999997E-2</v>
+        <v>5.8000000000000003E-2</v>
       </c>
       <c r="J5" s="12">
-        <v>5.5599999999999997E-2</v>
+        <v>5.8000000000000003E-2</v>
       </c>
       <c r="K5" s="12">
-        <v>5.5599999999999997E-2</v>
+        <v>5.8000000000000003E-2</v>
       </c>
       <c r="L5" s="12">
-        <v>5.5599999999999997E-2</v>
+        <v>5.8000000000000003E-2</v>
       </c>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.3">
@@ -2043,34 +2018,34 @@
         <v>13</v>
       </c>
       <c r="C7" s="12">
-        <v>0.312</v>
+        <v>0.36699999999999999</v>
       </c>
       <c r="D7" s="12">
-        <v>0.312</v>
+        <v>0.36699999999999999</v>
       </c>
       <c r="E7" s="12">
-        <v>0.312</v>
+        <v>0.36699999999999999</v>
       </c>
       <c r="F7" s="12">
-        <v>0.312</v>
+        <v>0.36699999999999999</v>
       </c>
       <c r="G7" s="12">
-        <v>0.312</v>
+        <v>0.36699999999999999</v>
       </c>
       <c r="H7" s="12">
-        <v>0.312</v>
+        <v>0.36699999999999999</v>
       </c>
       <c r="I7" s="12">
-        <v>0.312</v>
+        <v>0.36699999999999999</v>
       </c>
       <c r="J7" s="12">
-        <v>0.312</v>
+        <v>0.36699999999999999</v>
       </c>
       <c r="K7" s="12">
-        <v>0.312</v>
+        <v>0.36699999999999999</v>
       </c>
       <c r="L7" s="12">
-        <v>0.312</v>
+        <v>0.36699999999999999</v>
       </c>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.3">
@@ -2078,34 +2053,34 @@
         <v>14</v>
       </c>
       <c r="C8" s="12">
-        <v>8.9499999999999996E-2</v>
+        <v>0.1</v>
       </c>
       <c r="D8" s="12">
-        <v>8.9499999999999996E-2</v>
+        <v>0.1</v>
       </c>
       <c r="E8" s="12">
-        <v>8.9499999999999996E-2</v>
+        <v>0.1</v>
       </c>
       <c r="F8" s="12">
-        <v>8.9499999999999996E-2</v>
+        <v>0.1</v>
       </c>
       <c r="G8" s="12">
-        <v>8.9499999999999996E-2</v>
+        <v>0.1</v>
       </c>
       <c r="H8" s="12">
-        <v>8.9499999999999996E-2</v>
+        <v>0.1</v>
       </c>
       <c r="I8" s="12">
-        <v>8.9499999999999996E-2</v>
+        <v>0.1</v>
       </c>
       <c r="J8" s="12">
-        <v>8.9499999999999996E-2</v>
+        <v>0.1</v>
       </c>
       <c r="K8" s="12">
-        <v>8.9499999999999996E-2</v>
+        <v>0.1</v>
       </c>
       <c r="L8" s="12">
-        <v>8.9499999999999996E-2</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.3">
@@ -2232,34 +2207,34 @@
         <v>45</v>
       </c>
       <c r="C15" s="5">
-        <v>0.18099999999999999</v>
+        <v>0.39300000000000002</v>
       </c>
       <c r="D15" s="5">
-        <v>0.18099999999999999</v>
+        <v>0.39300000000000002</v>
       </c>
       <c r="E15" s="5">
-        <v>0.18099999999999999</v>
+        <v>0.39300000000000002</v>
       </c>
       <c r="F15" s="5">
-        <v>0.18099999999999999</v>
+        <v>0.39300000000000002</v>
       </c>
       <c r="G15" s="5">
-        <v>0.18099999999999999</v>
+        <v>0.39300000000000002</v>
       </c>
       <c r="H15" s="5">
-        <v>0.18099999999999999</v>
+        <v>0.39300000000000002</v>
       </c>
       <c r="I15" s="5">
-        <v>0.18099999999999999</v>
+        <v>0.39300000000000002</v>
       </c>
       <c r="J15" s="5">
-        <v>0.18099999999999999</v>
+        <v>0.39300000000000002</v>
       </c>
       <c r="K15" s="5">
-        <v>0.18099999999999999</v>
+        <v>0.39300000000000002</v>
       </c>
       <c r="L15" s="5">
-        <v>0.18099999999999999</v>
+        <v>0.39300000000000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>